<commit_message>
se hicieron cambios en la plantilla de Excel y se agregaron las celdas como constantes
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84DF3D6-2BD7-4ABF-A74D-CD91F10FC008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2334EB18-B76C-4B6F-86B3-89CE4AF5C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plantilla" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="365">
   <si>
     <t>Fecha</t>
   </si>
@@ -1111,6 +1111,27 @@
   </si>
   <si>
     <t>26/03/2024</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Lote / # de pedido / fecha de recepcion</t>
+  </si>
+  <si>
+    <t>Hierro</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Aros</t>
+  </si>
+  <si>
+    <t>Canastas</t>
+  </si>
+  <si>
+    <t>Castillos</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1299,13 +1320,8 @@
         <fgColor rgb="FF8EA9DB"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="8EA9DB"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1487,12 +1503,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1617,9 +1651,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1629,9 +1660,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1641,12 +1669,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1680,6 +1702,124 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1692,122 +1832,50 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2873,201 +2941,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:F30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29:P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.85546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="6" max="6" customWidth="true" width="10.140625"/>
-    <col min="7" max="7" customWidth="true" width="10.42578125"/>
-    <col min="8" max="8" customWidth="true" width="10.7109375"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5703125"/>
-    <col min="10" max="11" customWidth="true" width="10.5703125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625"/>
-    <col min="13" max="13" customWidth="true" width="11.42578125"/>
-    <col min="14" max="14" customWidth="true" width="12.85546875"/>
-    <col min="15" max="15" customWidth="true" width="26.42578125"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="104" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69" t="s">
+      <c r="E2" s="98"/>
+      <c r="F2" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69" t="s">
+      <c r="G2" s="98"/>
+      <c r="H2" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69" t="s">
+      <c r="I2" s="98"/>
+      <c r="J2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="69" t="s">
+      <c r="O2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="69"/>
+      <c r="P2" s="98"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="107">
+      <c r="A3" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="72" t="s">
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" t="s" s="107">
+      <c r="E3" s="106"/>
+      <c r="F3" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74">
+      <c r="G3" s="97"/>
+      <c r="H3" s="107">
         <v>8</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" t="s" s="107">
+      <c r="I3" s="97"/>
+      <c r="J3" s="95" t="s">
         <v>355</v>
       </c>
-      <c r="K3" s="75"/>
-      <c r="L3" s="73"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
-        <v>PC</v>
+        <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="101" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="65" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="101" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="65" t="s">
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="101" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="65" t="s">
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="101" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="67"/>
+      <c r="M4" s="103"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="69" t="s">
+      <c r="O4" s="98" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="69"/>
+      <c r="P4" s="98"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="84">
+      <c r="A5" s="82">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="84">
+      <c r="B5" s="83"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="82">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="89"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="87"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="107">
-        <v>123.0</v>
-      </c>
-      <c r="P5" s="76"/>
+      <c r="O5" s="95">
+        <v>123</v>
+      </c>
+      <c r="P5" s="99"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="90" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79" t="s">
+      <c r="B6" s="90"/>
+      <c r="C6" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80" t="s">
+      <c r="D6" s="91"/>
+      <c r="E6" s="92" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="81" t="s">
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="93" t="s">
         <v>296</v>
       </c>
-      <c r="L6" s="81"/>
-      <c r="M6" s="82" t="s">
+      <c r="L6" s="93"/>
+      <c r="M6" s="94" t="s">
         <v>299</v>
       </c>
-      <c r="N6" s="83" t="s">
+      <c r="N6" s="100" t="s">
         <v>300</v>
       </c>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="100"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3106,7 +3175,7 @@
       <c r="L7" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="M7" s="82"/>
+      <c r="M7" s="94"/>
       <c r="N7" s="26" t="s">
         <v>301</v>
       </c>
@@ -3774,14 +3843,14 @@
       <c r="P26" s="29"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -3791,276 +3860,272 @@
       <c r="O27" s="42"/>
       <c r="P27" s="42"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
+    <row r="28" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>358</v>
+      </c>
+      <c r="C28" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="D28" s="88" t="s">
         <v>306</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90" t="s">
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88" t="s">
         <v>314</v>
       </c>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90" t="s">
+      <c r="I28" s="88"/>
+      <c r="J28" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90" t="s">
+      <c r="K28" s="88"/>
+      <c r="L28" s="89" t="s">
+        <v>322</v>
+      </c>
+      <c r="M28" s="114" t="s">
+        <v>323</v>
+      </c>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="115"/>
+    </row>
+    <row r="29" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="H29" s="112">
+        <v>2</v>
+      </c>
+      <c r="I29" s="113"/>
+      <c r="J29" s="43" t="s">
+        <v>324</v>
+      </c>
+      <c r="K29" s="43" t="s">
+        <v>266</v>
+      </c>
+      <c r="L29" s="89"/>
+      <c r="M29" s="116">
+        <v>5</v>
+      </c>
+      <c r="N29" s="116"/>
+      <c r="O29" s="116"/>
+      <c r="P29" s="116"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="62" t="s">
+        <v>308</v>
+      </c>
+      <c r="E30" s="46">
+        <v>116</v>
+      </c>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="88" t="s">
+        <v>315</v>
+      </c>
+      <c r="I30" s="88"/>
+      <c r="J30" s="46">
+        <v>2</v>
+      </c>
+      <c r="K30" s="46">
+        <v>60</v>
+      </c>
+      <c r="L30" s="49"/>
+      <c r="M30" s="117">
+        <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
+        <v>4500</v>
+      </c>
+      <c r="N30" s="118"/>
+      <c r="O30" s="118"/>
+      <c r="P30" s="118"/>
+    </row>
+    <row r="31" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="63" t="s">
+        <v>309</v>
+      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="I31" s="46">
+        <v>2199</v>
+      </c>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="89" t="s">
+        <v>326</v>
+      </c>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+    </row>
+    <row r="32" spans="1:16" ht="36" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="63" t="s">
+        <v>310</v>
+      </c>
+      <c r="E32" s="46">
+        <v>33</v>
+      </c>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="71" t="s">
+        <v>317</v>
+      </c>
+      <c r="I32" s="46">
+        <v>14</v>
+      </c>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+    </row>
+    <row r="33" spans="1:16" ht="36" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="65"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="E33" s="46">
+        <v>2</v>
+      </c>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="72" t="s">
+        <v>318</v>
+      </c>
+      <c r="I33" s="70" t="s">
+        <v>319</v>
+      </c>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="49">
+        <v>34</v>
+      </c>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+    </row>
+    <row r="34" spans="1:16" ht="36" x14ac:dyDescent="0.25">
+      <c r="A34" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="63" t="s">
+        <v>312</v>
+      </c>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="108" t="s">
+        <v>329</v>
+      </c>
+      <c r="I34" s="111"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="48" t="s">
+        <v>328</v>
+      </c>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
+        <v>298</v>
+      </c>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="E35" s="46">
+        <f>E30+E31-E32-E33-E34</f>
+        <v>81</v>
+      </c>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="I35" s="68" t="s">
+        <v>331</v>
+      </c>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="49">
+        <v>0</v>
+      </c>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
+        <v>360</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="108" t="s">
+        <v>327</v>
+      </c>
+      <c r="E36" s="109"/>
+      <c r="F36" s="109"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="76" t="s">
         <v>321</v>
       </c>
-      <c r="J28" s="90"/>
-      <c r="K28" s="93" t="s">
-        <v>322</v>
-      </c>
-      <c r="L28" s="43" t="s">
-        <v>323</v>
-      </c>
-      <c r="M28" s="43"/>
-      <c r="N28" s="90" t="s">
-        <v>329</v>
-      </c>
-      <c r="O28" s="90"/>
-      <c r="P28" s="90"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="45" t="s">
-        <v>307</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>295</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="E29" s="91">
-        <v>2</v>
-      </c>
-      <c r="F29" s="92"/>
-      <c r="G29" s="43" t="s">
-        <v>324</v>
-      </c>
-      <c r="H29" s="43" t="s">
-        <v>266</v>
-      </c>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="47">
-        <v>5</v>
-      </c>
-      <c r="M29" s="47"/>
-      <c r="N29" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="O29" s="90" t="s">
-        <v>331</v>
-      </c>
-      <c r="P29" s="90"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
-        <v>308</v>
-      </c>
-      <c r="B30" s="47">
-        <v>116</v>
-      </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="47">
-        <v>2</v>
-      </c>
-      <c r="H30" s="47">
-        <v>60</v>
-      </c>
-      <c r="I30" s="47" t="s">
-        <v>325</v>
-      </c>
-      <c r="J30" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="K30" s="51"/>
-      <c r="L30" s="47">
-        <f>IF(L29=0,0,((L29*1000)/1.25)+500)</f>
-        <v>4500</v>
-      </c>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="O30" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="P30" s="91"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
-        <v>309</v>
-      </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="90" t="s">
-        <v>315</v>
-      </c>
-      <c r="F31" s="90"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47" t="s">
-        <v>325</v>
-      </c>
-      <c r="J31" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="K31" s="93" t="s">
-        <v>326</v>
-      </c>
-      <c r="L31" s="52"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="43" t="s">
-        <v>332</v>
-      </c>
-      <c r="O31" s="94">
-        <v>0</v>
-      </c>
-      <c r="P31" s="94"/>
-    </row>
-    <row r="32" spans="1:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="A32" s="48" t="s">
-        <v>310</v>
-      </c>
-      <c r="B32" s="47">
-        <v>33</v>
-      </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="F32" s="47">
-        <v>2199</v>
-      </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47" t="s">
-        <v>325</v>
-      </c>
-      <c r="J32" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="K32" s="93"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="O32" s="90" t="s">
-        <v>331</v>
-      </c>
-      <c r="P32" s="90"/>
-    </row>
-    <row r="33" spans="1:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
-        <v>311</v>
-      </c>
-      <c r="B33" s="47">
-        <v>2</v>
-      </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="49" t="s">
-        <v>317</v>
-      </c>
-      <c r="F33" s="47">
-        <v>14</v>
-      </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="90" t="s">
-        <v>327</v>
-      </c>
-      <c r="J33" s="90"/>
-      <c r="K33" s="51">
-        <v>34</v>
-      </c>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="O33" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="P33" s="91"/>
-    </row>
-    <row r="34" spans="1:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
-        <v>312</v>
-      </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="91" t="s">
-        <v>318</v>
-      </c>
-      <c r="F34" s="91"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="43" t="s">
-        <v>332</v>
-      </c>
-      <c r="O34" s="91"/>
-      <c r="P34" s="91"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
-        <v>313</v>
-      </c>
-      <c r="B35" s="47">
-        <f>B30+B31-B32-B33-B34</f>
-        <v>81</v>
-      </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="97" t="s">
-        <v>319</v>
-      </c>
-      <c r="F35" s="98"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="91"/>
-      <c r="K35" s="51">
-        <v>0</v>
-      </c>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="91"/>
-      <c r="P35" s="91"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
+      <c r="K36" s="77"/>
       <c r="L36" s="42"/>
       <c r="M36" s="42"/>
       <c r="N36" s="42"/>
@@ -4068,242 +4133,312 @@
       <c r="P36" s="42"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="95" t="s">
+      <c r="A37" s="45" t="s">
+        <v>361</v>
+      </c>
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="74" t="s">
+        <v>362</v>
+      </c>
+      <c r="E37" s="110"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="I37" s="73">
+        <v>0</v>
+      </c>
+      <c r="J37" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="K37" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="45" t="s">
+        <v>361</v>
+      </c>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="74" t="s">
+        <v>363</v>
+      </c>
+      <c r="E38" s="110"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="K38" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="42"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="78"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="74" t="s">
+        <v>364</v>
+      </c>
+      <c r="E39" s="74"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="K39" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="42"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="78"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="79" t="s">
         <v>333</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="96" t="s">
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="80" t="s">
         <v>334</v>
       </c>
-      <c r="J37" s="96"/>
-      <c r="K37" s="96"/>
-      <c r="L37" s="96"/>
-      <c r="M37" s="96"/>
-      <c r="N37" s="96"/>
-      <c r="O37" s="96"/>
-      <c r="P37" s="96"/>
-    </row>
-    <row r="38" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
+      <c r="J41" s="80"/>
+      <c r="K41" s="80"/>
+      <c r="L41" s="80"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="80"/>
+      <c r="O41" s="80"/>
+      <c r="P41" s="80"/>
+    </row>
+    <row r="42" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="50" t="s">
         <v>335</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B42" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C42" s="52" t="s">
         <v>350</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D42" s="52" t="s">
         <v>351</v>
       </c>
-      <c r="E38" s="56" t="s">
+      <c r="E42" s="52" t="s">
         <v>352</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F42" s="52" t="s">
         <v>353</v>
       </c>
-      <c r="G38" s="56" t="s">
+      <c r="G42" s="52" t="s">
         <v>337</v>
       </c>
-      <c r="H38" s="54" t="s">
+      <c r="H42" s="50" t="s">
         <v>338</v>
       </c>
-      <c r="I38" s="55" t="s">
+      <c r="I42" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="J38" s="55" t="s">
+      <c r="J42" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="K38" s="55" t="s">
+      <c r="K42" s="51" t="s">
         <v>341</v>
       </c>
-      <c r="L38" s="55" t="s">
+      <c r="L42" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="M38" s="55" t="s">
+      <c r="M42" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="N38" s="55" t="s">
+      <c r="N42" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="O38" s="55" t="s">
+      <c r="O42" s="51" t="s">
         <v>345</v>
       </c>
-      <c r="P38" s="55" t="s">
+      <c r="P42" s="51" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="57">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="53">
         <f>+IFERROR((M26/D26),0)</f>
         <v>10000</v>
       </c>
-      <c r="B39" s="58">
+      <c r="B43" s="54">
         <f>D5-A5</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="C39" s="64">
-        <f>(HOUR(B39)*60)+(MINUTE(B39))-60</f>
+      <c r="C43" s="60">
+        <f>(HOUR(B43)*60)+(MINUTE(B43))-60</f>
         <v>660</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D43" s="46">
         <f>+COUNTA(B8:B25)*60</f>
         <v>0</v>
       </c>
-      <c r="E39" s="59">
-        <f>IFERROR(C39/D39,0)</f>
+      <c r="E43" s="55">
+        <f>IFERROR(C43/D43,0)</f>
         <v>0</v>
       </c>
-      <c r="F39" s="47">
+      <c r="F43" s="46">
         <v>5</v>
       </c>
-      <c r="G39" s="47">
+      <c r="G43" s="46">
         <v>7</v>
       </c>
-      <c r="H39" s="57">
-        <f>IFERROR(H5/F39,0)</f>
+      <c r="H43" s="53">
+        <f>IFERROR(H5/F43,0)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="60">
+      <c r="I43" s="56">
         <f>IFERROR(E26/$M$26,0)</f>
         <v>0.26</v>
       </c>
-      <c r="J39" s="60">
+      <c r="J43" s="56">
         <f>IFERROR(F26/$M$26,0)</f>
         <v>0.25333333333333335</v>
       </c>
-      <c r="K39" s="60">
+      <c r="K43" s="56">
         <f>IFERROR(G26/$M$26,0)</f>
         <v>0.24666666666666667</v>
       </c>
-      <c r="L39" s="60">
+      <c r="L43" s="56">
         <f>IFERROR(H26/$M$26,0)</f>
         <v>0.24</v>
       </c>
-      <c r="M39" s="60">
-        <f>IFERROR(K33/$M$26,0)</f>
+      <c r="M43" s="56">
+        <f>IFERROR(L33/$M$26,0)</f>
         <v>2.2666666666666666E-4</v>
       </c>
-      <c r="N39" s="60">
+      <c r="N43" s="56">
         <f>IFERROR(I26/$M$26,0)</f>
         <v>0.27333333333333332</v>
       </c>
-      <c r="O39" s="60">
-        <f>IFERROR(D33/$M$26,0)</f>
+      <c r="O43" s="56">
+        <f>IFERROR(G33/$M$26,0)</f>
         <v>0</v>
       </c>
-      <c r="P39" s="60">
+      <c r="P43" s="56">
         <f>IFERROR(K26/$M$26,0)</f>
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="61"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="62" t="s">
+    <row r="44" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="58" t="s">
         <v>347</v>
       </c>
-      <c r="J40" s="62" t="s">
+      <c r="J44" s="58" t="s">
         <v>348</v>
       </c>
-      <c r="K40" s="62" t="s">
+      <c r="K44" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="L40" s="62" t="s">
+      <c r="L44" s="58" t="s">
         <v>349</v>
       </c>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
-      <c r="P40" s="61"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="61"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="60">
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+      <c r="P44" s="57"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="56">
         <f>IFERROR(L26/$M$26,0)</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="J41" s="60">
-        <f>IFERROR(E29/$M$26,0)</f>
+      <c r="J45" s="56">
+        <f>IFERROR(H29/$M$26,0)</f>
         <v>1.3333333333333333E-5</v>
       </c>
-      <c r="K41" s="63">
-        <f>IFERROR(L30/D26,0)</f>
+      <c r="K45" s="59">
+        <f>IFERROR(M30/D26,0)</f>
         <v>300</v>
       </c>
-      <c r="L41" s="63">
+      <c r="L45" s="59">
         <f>IFERROR(H26/D26,0)</f>
         <v>2400</v>
       </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="61"/>
-      <c r="O41" s="61"/>
-      <c r="P41" s="61"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+      <c r="P45" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="I37:P37"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="H4:K4"/>
+  <mergeCells count="56">
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="L31:L32"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:G4"/>
@@ -4319,6 +4454,40 @@
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="I41:P41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{AEF5EDB9-E736-4AB4-A9AF-637FA36B9F1A}">
@@ -4330,10 +4499,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I3" xr:uid="{9561FAB1-7A4F-4FA7-887F-AF2562E1B9CB}">
       <formula1>INDIRECT($F$3)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E35:F35" xr:uid="{FB065D7C-B20C-4A8C-BBDD-59A3B275D760}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I33" xr:uid="{FB065D7C-B20C-4A8C-BBDD-59A3B275D760}">
       <formula1>"Empleado 1, Empleado2, Empleado 3, Empleado 4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N30:O30 N33:O33" xr:uid="{2BE9F060-0544-492D-BFC4-E4092DFF73D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H36:I36 H38:I38" xr:uid="{2BE9F060-0544-492D-BFC4-E4092DFF73D0}">
       <formula1>"Maquina 1, Maquina 2, Maquina 3, Maquina 4, Maquina 5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4351,17 +4520,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.28515625"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
@@ -4611,7 +4780,7 @@
       <c r="O4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="S4" t="s" s="0">
+      <c r="S4" t="s">
         <v>62</v>
       </c>
       <c r="U4" s="8" t="s">
@@ -4678,7 +4847,7 @@
       <c r="O5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S5" t="s" s="0">
+      <c r="S5" t="s">
         <v>71</v>
       </c>
       <c r="U5" s="8" t="s">

</xml_diff>

<commit_message>
Se pasaron los metodos a CargaDatosProceso, creacion de diferentes DTO y Util para la comunicacion con persistencia
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2334EB18-B76C-4B6F-86B3-89CE4AF5C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4502A7BE-811F-4EDF-807E-A3553490B99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1763,6 +1763,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1802,53 +1811,44 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2943,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29:P29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,24 +2966,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="98" t="s">
@@ -3023,61 +3023,61 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="99" t="s">
         <v>357</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="106" t="s">
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="95" t="s">
+      <c r="E3" s="107"/>
+      <c r="F3" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="97"/>
-      <c r="H3" s="107">
+      <c r="G3" s="108"/>
+      <c r="H3" s="109">
         <v>8</v>
       </c>
-      <c r="I3" s="97"/>
-      <c r="J3" s="95" t="s">
+      <c r="I3" s="108"/>
+      <c r="J3" s="99" t="s">
         <v>355</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="97"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="108"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="107"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="102" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="101" t="s">
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="101" t="s">
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="102" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="101" t="s">
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="102" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="103"/>
+      <c r="M4" s="104"/>
       <c r="N4" s="3"/>
       <c r="O4" s="98" t="s">
         <v>263</v>
@@ -3085,58 +3085,58 @@
       <c r="P4" s="98"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="82">
+      <c r="A5" s="85">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="82">
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="85">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="87"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="90"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="95">
+      <c r="O5" s="99">
         <v>123</v>
       </c>
-      <c r="P5" s="99"/>
+      <c r="P5" s="100"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="93" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91" t="s">
+      <c r="B6" s="93"/>
+      <c r="C6" s="94" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="91"/>
-      <c r="E6" s="92" t="s">
+      <c r="D6" s="94"/>
+      <c r="E6" s="95" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="93" t="s">
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="96" t="s">
         <v>296</v>
       </c>
-      <c r="L6" s="93"/>
-      <c r="M6" s="94" t="s">
+      <c r="L6" s="96"/>
+      <c r="M6" s="97" t="s">
         <v>299</v>
       </c>
-      <c r="N6" s="100" t="s">
+      <c r="N6" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="101"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3175,7 +3175,7 @@
       <c r="L7" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="M7" s="94"/>
+      <c r="M7" s="97"/>
       <c r="N7" s="26" t="s">
         <v>301</v>
       </c>
@@ -3870,21 +3870,21 @@
       <c r="C28" s="69" t="s">
         <v>359</v>
       </c>
-      <c r="D28" s="88" t="s">
+      <c r="D28" s="91" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88" t="s">
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91" t="s">
         <v>314</v>
       </c>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88" t="s">
+      <c r="I28" s="91"/>
+      <c r="J28" s="91" t="s">
         <v>320</v>
       </c>
-      <c r="K28" s="88"/>
-      <c r="L28" s="89" t="s">
+      <c r="K28" s="91"/>
+      <c r="L28" s="92" t="s">
         <v>322</v>
       </c>
       <c r="M28" s="114" t="s">
@@ -3920,7 +3920,7 @@
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="89"/>
+      <c r="L29" s="92"/>
       <c r="M29" s="116">
         <v>5</v>
       </c>
@@ -3942,10 +3942,10 @@
       </c>
       <c r="F30" s="46"/>
       <c r="G30" s="46"/>
-      <c r="H30" s="88" t="s">
+      <c r="H30" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="I30" s="88"/>
+      <c r="I30" s="91"/>
       <c r="J30" s="46">
         <v>2</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="J31" s="46"/>
       <c r="K31" s="46"/>
-      <c r="L31" s="89" t="s">
+      <c r="L31" s="92" t="s">
         <v>326</v>
       </c>
       <c r="M31" s="42"/>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="J32" s="46"/>
       <c r="K32" s="46"/>
-      <c r="L32" s="89"/>
+      <c r="L32" s="92"/>
       <c r="M32" s="42"/>
       <c r="N32" s="42"/>
       <c r="O32" s="42"/>
@@ -4059,7 +4059,7 @@
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
-      <c r="H34" s="108" t="s">
+      <c r="H34" s="82" t="s">
         <v>329</v>
       </c>
       <c r="I34" s="111"/>
@@ -4110,12 +4110,12 @@
       </c>
       <c r="B36" s="65"/>
       <c r="C36" s="65"/>
-      <c r="D36" s="108" t="s">
+      <c r="D36" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="E36" s="109"/>
-      <c r="F36" s="109"/>
-      <c r="G36" s="109"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
       <c r="H36" s="46" t="s">
         <v>8</v>
       </c>
@@ -4141,7 +4141,7 @@
       <c r="D37" s="74" t="s">
         <v>362</v>
       </c>
-      <c r="E37" s="110"/>
+      <c r="E37" s="84"/>
       <c r="F37" s="75"/>
       <c r="G37" s="75"/>
       <c r="H37" s="43" t="s">
@@ -4171,7 +4171,7 @@
       <c r="D38" s="74" t="s">
         <v>363</v>
       </c>
-      <c r="E38" s="110"/>
+      <c r="E38" s="84"/>
       <c r="F38" s="75"/>
       <c r="G38" s="75"/>
       <c r="H38" s="46" t="s">

</xml_diff>

<commit_message>
Se crearon DTO necesarios para el mapeo de los objetos de Dominio, a la vez que se obtienen todos los valores del formato de Excel
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4502A7BE-811F-4EDF-807E-A3553490B99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDDDA99-3EE8-4DC1-8D94-9A7E43E732CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="387">
   <si>
     <t>Fecha</t>
   </si>
@@ -960,9 +960,6 @@
     <t>CONTROL DE:</t>
   </si>
   <si>
-    <t>CEMENTO</t>
-  </si>
-  <si>
     <t>Saldo inicial</t>
   </si>
   <si>
@@ -1005,9 +1002,6 @@
     <t>Registros contables</t>
   </si>
   <si>
-    <t>Cemento Pulir</t>
-  </si>
-  <si>
     <t>Desmoldante</t>
   </si>
   <si>
@@ -1017,15 +1011,9 @@
     <t>Documento</t>
   </si>
   <si>
-    <t>Cemento Kilos Pulida</t>
-  </si>
-  <si>
     <t>HIERRO</t>
   </si>
   <si>
-    <t>Pulir M50</t>
-  </si>
-  <si>
     <t>Traslado de Mezcla</t>
   </si>
   <si>
@@ -1132,6 +1120,84 @@
   </si>
   <si>
     <t>Castillos</t>
+  </si>
+  <si>
+    <t>CEMENTO Bultos 50 k</t>
+  </si>
+  <si>
+    <t>CEMENTO Bultos 42,5 k</t>
+  </si>
+  <si>
+    <t>CEMENTO K</t>
+  </si>
+  <si>
+    <t>Acelerante</t>
+  </si>
+  <si>
+    <t>Tiempos Parada Maquina</t>
+  </si>
+  <si>
+    <t>Almacenamiento</t>
+  </si>
+  <si>
+    <t>Asesoria u organización</t>
+  </si>
+  <si>
+    <t>Otras Producciones</t>
+  </si>
+  <si>
+    <t>Falta de mezcla</t>
+  </si>
+  <si>
+    <t>Falta de MP</t>
+  </si>
+  <si>
+    <t>Organización anillo - formaletas</t>
+  </si>
+  <si>
+    <t>Pintar Productos</t>
+  </si>
+  <si>
+    <t>Programa de gerencia</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Contador De Agua</t>
+  </si>
+  <si>
+    <t>Lectura Inicial</t>
+  </si>
+  <si>
+    <t>Lectura Final</t>
+  </si>
+  <si>
+    <t>Recurso Humano Producción</t>
+  </si>
+  <si>
+    <t>Mezclador</t>
+  </si>
+  <si>
+    <t>Aux Mezclador</t>
+  </si>
+  <si>
+    <t>Operario</t>
+  </si>
+  <si>
+    <t>Aux Operario</t>
+  </si>
+  <si>
+    <t>Pulidor</t>
+  </si>
+  <si>
+    <t>Auxiliar</t>
+  </si>
+  <si>
+    <t>Cemento Kilos Pulida Dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1209,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1213,6 +1279,13 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1526,7 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1651,9 +1724,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1662,9 +1732,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1739,15 +1806,52 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1757,99 +1861,105 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1859,22 +1969,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2943,8 +3050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:G35"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,184 +3066,194 @@
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.5703125" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
-        <v>354</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
+      <c r="A1" s="83" t="s">
+        <v>350</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98" t="s">
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98" t="s">
+      <c r="E2" s="111"/>
+      <c r="F2" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98" t="s">
+      <c r="G2" s="111"/>
+      <c r="H2" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98" t="s">
+      <c r="I2" s="111"/>
+      <c r="J2" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="98" t="s">
+      <c r="O2" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="98"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="99" t="s">
-        <v>357</v>
-      </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="107" t="s">
+      <c r="A3" s="118" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3" s="119"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="107"/>
-      <c r="F3" s="99" t="s">
+      <c r="E3" s="115"/>
+      <c r="F3" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="109">
+      <c r="G3" s="120"/>
+      <c r="H3" s="121">
         <v>8</v>
       </c>
-      <c r="I3" s="108"/>
-      <c r="J3" s="99" t="s">
-        <v>355</v>
-      </c>
-      <c r="K3" s="110"/>
-      <c r="L3" s="108"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="118" t="s">
+        <v>351</v>
+      </c>
+      <c r="K3" s="122"/>
+      <c r="L3" s="120"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="102" t="s">
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="102" t="s">
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="112" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="102" t="s">
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="112" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="104"/>
+      <c r="M4" s="114"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="98" t="s">
+      <c r="O4" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="98"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="85">
+      <c r="A5" s="94">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="85">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="94">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="90"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="99"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="99">
+      <c r="O5" s="116">
         <v>123</v>
       </c>
-      <c r="P5" s="100"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="102" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="94" t="s">
+      <c r="B6" s="102"/>
+      <c r="C6" s="103" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="95" t="s">
+      <c r="D6" s="103"/>
+      <c r="E6" s="105" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="96" t="s">
+      <c r="F6" s="106"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="108" t="s">
         <v>296</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="97" t="s">
+      <c r="J6" s="109"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="104" t="s">
         <v>299</v>
       </c>
-      <c r="N6" s="101" t="s">
+      <c r="M6" s="128" t="s">
         <v>300</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="117" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q6" s="117"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3163,27 +3280,30 @@
       <c r="H7" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="J7" s="33" t="s">
-        <v>295</v>
+      <c r="I7" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>298</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>297</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="M7" s="97"/>
+        <v>364</v>
+      </c>
+      <c r="L7" s="104"/>
+      <c r="M7" s="26" t="s">
+        <v>301</v>
+      </c>
       <c r="N7" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="P7" s="26" t="s">
         <v>303</v>
+      </c>
+      <c r="P7" s="72">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="73" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3209,30 +3329,33 @@
       <c r="H8" s="34">
         <v>5000</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="37">
         <v>5000</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="37">
         <v>5000</v>
       </c>
       <c r="K8" s="37">
         <v>5000</v>
       </c>
-      <c r="L8" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M8" s="40">
-        <f t="shared" ref="M8:M25" si="0">SUM(E8:H8)</f>
+      <c r="L8" s="40">
+        <f t="shared" ref="L8:L25" si="0">SUM(E8:H8)</f>
         <v>20000</v>
       </c>
-      <c r="N8" s="29">
+      <c r="M8" s="29">
         <v>1</v>
       </c>
-      <c r="O8" s="29" t="s">
-        <v>356</v>
-      </c>
-      <c r="P8" s="29">
+      <c r="N8" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="O8" s="29">
         <v>1</v>
+      </c>
+      <c r="P8" s="72">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="73" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3258,30 +3381,33 @@
       <c r="H9" s="34">
         <v>5000</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="37">
         <v>5000</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="37">
         <v>5000</v>
       </c>
       <c r="K9" s="37">
         <v>5000</v>
       </c>
-      <c r="L9" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M9" s="40">
+      <c r="L9" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="N9" s="29">
+      <c r="M9" s="29">
         <v>1</v>
       </c>
-      <c r="O9" s="29" t="s">
-        <v>356</v>
-      </c>
-      <c r="P9" s="29">
+      <c r="N9" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="O9" s="29">
         <v>1</v>
+      </c>
+      <c r="P9" s="72">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="73" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3305,30 +3431,33 @@
       <c r="H10" s="34">
         <v>5000</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="37">
         <v>5000</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="37">
         <v>5000</v>
       </c>
       <c r="K10" s="37">
         <v>5000</v>
       </c>
-      <c r="L10" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M10" s="40">
+      <c r="L10" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="N10" s="29">
+      <c r="M10" s="29">
         <v>1</v>
       </c>
-      <c r="O10" s="29" t="s">
-        <v>356</v>
-      </c>
-      <c r="P10" s="29">
+      <c r="N10" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="O10" s="29">
         <v>1</v>
+      </c>
+      <c r="P10" s="72">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="73" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -3352,27 +3481,30 @@
       <c r="H11" s="34">
         <v>5000</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="37">
         <v>5000</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="37">
         <v>5000</v>
       </c>
       <c r="K11" s="37">
         <v>5000</v>
       </c>
-      <c r="L11" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M11" s="40">
+      <c r="L11" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
+      <c r="M11" s="29"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P11" s="72">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="73" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>5</v>
       </c>
@@ -3393,25 +3525,28 @@
       <c r="H12" s="34">
         <v>5000</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="37">
         <v>5000</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="37">
         <v>5000</v>
       </c>
       <c r="K12" s="37">
         <v>5000</v>
       </c>
-      <c r="L12" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M12" s="40">
+      <c r="L12" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
+      <c r="M12" s="29"/>
       <c r="N12" s="29"/>
       <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
+      <c r="P12" s="72">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="74" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -3434,25 +3569,28 @@
       <c r="H13" s="34">
         <v>5000</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="37">
         <v>5000</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="37">
         <v>5000</v>
       </c>
       <c r="K13" s="37">
         <v>5000</v>
       </c>
-      <c r="L13" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M13" s="40">
+      <c r="L13" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
+      <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="P13" s="72">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="73" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
@@ -3475,25 +3613,28 @@
       <c r="H14" s="34">
         <v>5000</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="37">
         <v>5000</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="37">
         <v>5000</v>
       </c>
       <c r="K14" s="37">
         <v>5000</v>
       </c>
-      <c r="L14" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M14" s="40">
+      <c r="L14" s="40">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
+      <c r="M14" s="29"/>
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
+      <c r="P14" s="72">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="73" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
@@ -3516,25 +3657,28 @@
       <c r="H15" s="34">
         <v>1000</v>
       </c>
-      <c r="I15" s="34">
-        <v>6000</v>
-      </c>
-      <c r="J15" s="34">
+      <c r="I15" s="37">
+        <v>5000</v>
+      </c>
+      <c r="J15" s="37">
         <v>5000</v>
       </c>
       <c r="K15" s="37">
         <v>5000</v>
       </c>
-      <c r="L15" s="37">
-        <v>5000</v>
-      </c>
-      <c r="M15" s="40">
+      <c r="L15" s="40">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
+      <c r="M15" s="29"/>
       <c r="N15" s="29"/>
       <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
+      <c r="P15" s="72">
+        <v>17</v>
+      </c>
+      <c r="Q15" s="73" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
@@ -3549,19 +3693,20 @@
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="40">
+      <c r="I16" s="37"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" s="72"/>
+      <c r="Q16" s="73"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>10</v>
       </c>
@@ -3574,19 +3719,20 @@
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="40">
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P17" s="72"/>
+      <c r="Q17" s="73"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>11</v>
       </c>
@@ -3599,19 +3745,20 @@
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="40">
+      <c r="I18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="72"/>
+      <c r="Q18" s="73"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>12</v>
       </c>
@@ -3624,19 +3771,20 @@
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="40">
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M19" s="29"/>
       <c r="N19" s="29"/>
       <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P19" s="72"/>
+      <c r="Q19" s="73"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>13</v>
       </c>
@@ -3649,19 +3797,20 @@
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="40">
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M20" s="29"/>
       <c r="N20" s="29"/>
       <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P20" s="72"/>
+      <c r="Q20" s="73"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>14</v>
       </c>
@@ -3674,19 +3823,20 @@
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="40">
+      <c r="I21" s="37"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M21" s="29"/>
       <c r="N21" s="29"/>
       <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P21" s="72"/>
+      <c r="Q21" s="73"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>15</v>
       </c>
@@ -3699,19 +3849,20 @@
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="40">
+      <c r="L22" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M22" s="29"/>
       <c r="N22" s="29"/>
       <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P22" s="72"/>
+      <c r="Q22" s="73"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>16</v>
       </c>
@@ -3724,19 +3875,20 @@
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="40">
+      <c r="L23" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P23" s="72"/>
+      <c r="Q23" s="73"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>17</v>
       </c>
@@ -3749,19 +3901,20 @@
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="40">
+      <c r="L24" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M24" s="29"/>
       <c r="N24" s="29"/>
       <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>18</v>
       </c>
@@ -3774,19 +3927,20 @@
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="40">
+      <c r="L25" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M25" s="29"/>
       <c r="N25" s="29"/>
       <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>267</v>
       </c>
@@ -3796,7 +3950,7 @@
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="32">
-        <f t="shared" ref="D26:N26" si="1">SUM(D8:D25)</f>
+        <f t="shared" ref="D26:G26" si="1">SUM(D8:D25)</f>
         <v>15</v>
       </c>
       <c r="E26" s="35">
@@ -3812,45 +3966,43 @@
         <v>37000</v>
       </c>
       <c r="H26" s="35">
-        <f>SUM(H8:H25)</f>
+        <f t="shared" ref="H26:M26" si="2">SUM(H8:H25)</f>
         <v>36000</v>
       </c>
-      <c r="I26" s="35">
-        <f t="shared" ref="I26:J26" si="2">SUM(I8:I25)</f>
-        <v>41000</v>
-      </c>
-      <c r="J26" s="35">
+      <c r="I26" s="39">
         <f t="shared" si="2"/>
         <v>40000</v>
       </c>
+      <c r="J26" s="39">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
       <c r="K26" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40000</v>
       </c>
-      <c r="L26" s="39">
-        <f t="shared" si="1"/>
-        <v>40000</v>
-      </c>
-      <c r="M26" s="41">
-        <f t="shared" si="1"/>
+      <c r="L26" s="41">
+        <f t="shared" si="2"/>
         <v>150000</v>
       </c>
-      <c r="N26" s="29">
-        <f t="shared" si="1"/>
+      <c r="M26" s="29">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="N26" s="29"/>
       <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="64"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -3859,587 +4011,617 @@
       <c r="N27" s="42"/>
       <c r="O27" s="42"/>
       <c r="P27" s="42"/>
-    </row>
-    <row r="28" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="Q27" s="42"/>
+    </row>
+    <row r="28" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>358</v>
-      </c>
-      <c r="C28" s="69" t="s">
-        <v>359</v>
-      </c>
-      <c r="D28" s="91" t="s">
+        <v>354</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>355</v>
+      </c>
+      <c r="D28" s="100" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91" t="s">
-        <v>314</v>
-      </c>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91" t="s">
-        <v>320</v>
-      </c>
-      <c r="K28" s="91"/>
-      <c r="L28" s="92" t="s">
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100" t="s">
+        <v>313</v>
+      </c>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100" t="s">
+        <v>319</v>
+      </c>
+      <c r="K28" s="100"/>
+      <c r="L28" s="101" t="s">
+        <v>385</v>
+      </c>
+      <c r="M28" s="100" t="s">
+        <v>321</v>
+      </c>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="100"/>
+    </row>
+    <row r="29" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="67" t="s">
+        <v>362</v>
+      </c>
+      <c r="F29" s="67" t="s">
+        <v>361</v>
+      </c>
+      <c r="G29" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="H29" s="125">
+        <v>2</v>
+      </c>
+      <c r="I29" s="126"/>
+      <c r="J29" s="43" t="s">
         <v>322</v>
-      </c>
-      <c r="M28" s="114" t="s">
-        <v>323</v>
-      </c>
-      <c r="N28" s="115"/>
-      <c r="O28" s="115"/>
-      <c r="P28" s="115"/>
-    </row>
-    <row r="29" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>290</v>
-      </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="44" t="s">
-        <v>307</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>295</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="H29" s="112">
-        <v>2</v>
-      </c>
-      <c r="I29" s="113"/>
-      <c r="J29" s="43" t="s">
-        <v>324</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="92"/>
-      <c r="M29" s="116">
-        <v>5</v>
-      </c>
-      <c r="N29" s="116"/>
-      <c r="O29" s="116"/>
-      <c r="P29" s="116"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="L29" s="101"/>
+      <c r="M29" s="131">
+        <v>8</v>
+      </c>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
+      <c r="Q29" s="131"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="62" t="s">
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="60" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" s="45">
+        <v>116</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>386</v>
+      </c>
+      <c r="G30" s="45"/>
+      <c r="H30" s="100" t="s">
+        <v>314</v>
+      </c>
+      <c r="I30" s="100"/>
+      <c r="J30" s="45">
+        <v>2</v>
+      </c>
+      <c r="K30" s="45">
+        <v>60</v>
+      </c>
+      <c r="L30" s="47"/>
+      <c r="M30" s="131">
+        <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
+        <v>6900</v>
+      </c>
+      <c r="N30" s="131"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
+      <c r="Q30" s="131"/>
+    </row>
+    <row r="31" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="61" t="s">
         <v>308</v>
       </c>
-      <c r="E30" s="46">
-        <v>116</v>
-      </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="91" t="s">
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="69" t="s">
         <v>315</v>
       </c>
-      <c r="I30" s="91"/>
-      <c r="J30" s="46">
+      <c r="I31" s="45">
+        <v>2199</v>
+      </c>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="84" t="s">
+        <v>378</v>
+      </c>
+      <c r="N31" s="85"/>
+      <c r="O31" s="85"/>
+      <c r="P31" s="85"/>
+      <c r="Q31" s="85"/>
+    </row>
+    <row r="32" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+      <c r="A32" s="44" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="E32" s="45">
+        <v>33</v>
+      </c>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="I32" s="45">
+        <v>14</v>
+      </c>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="79" t="s">
+        <v>379</v>
+      </c>
+      <c r="N32" s="79"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="81"/>
+      <c r="Q32" s="82"/>
+    </row>
+    <row r="33" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+      <c r="A33" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="E33" s="45">
         <v>2</v>
       </c>
-      <c r="K30" s="46">
-        <v>60</v>
-      </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="117">
-        <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
-        <v>4500</v>
-      </c>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="118"/>
-    </row>
-    <row r="31" spans="1:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>292</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="63" t="s">
-        <v>309</v>
-      </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="71" t="s">
-        <v>316</v>
-      </c>
-      <c r="I31" s="46">
-        <v>2199</v>
-      </c>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="92" t="s">
-        <v>326</v>
-      </c>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-    </row>
-    <row r="32" spans="1:16" ht="36" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
-        <v>293</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="63" t="s">
-        <v>310</v>
-      </c>
-      <c r="E32" s="46">
-        <v>33</v>
-      </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="71" t="s">
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="70" t="s">
         <v>317</v>
       </c>
-      <c r="I32" s="46">
-        <v>14</v>
-      </c>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="92"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-    </row>
-    <row r="33" spans="1:16" ht="36" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="63" t="s">
+      <c r="I33" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="79" t="s">
+        <v>380</v>
+      </c>
+      <c r="N33" s="79"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="81"/>
+      <c r="Q33" s="82"/>
+    </row>
+    <row r="34" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="61" t="s">
         <v>311</v>
       </c>
-      <c r="E33" s="46">
-        <v>2</v>
-      </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="I33" s="70" t="s">
-        <v>319</v>
-      </c>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="49">
-        <v>34</v>
-      </c>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-    </row>
-    <row r="34" spans="1:16" ht="36" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
-        <v>295</v>
-      </c>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="63" t="s">
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="123" t="s">
+        <v>325</v>
+      </c>
+      <c r="I34" s="124"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="79" t="s">
+        <v>381</v>
+      </c>
+      <c r="N34" s="79"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="82"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="60" t="s">
         <v>312</v>
       </c>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="82" t="s">
-        <v>329</v>
-      </c>
-      <c r="I34" s="111"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="48" t="s">
-        <v>328</v>
-      </c>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
-        <v>298</v>
-      </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="62" t="s">
-        <v>313</v>
-      </c>
-      <c r="E35" s="46">
+      <c r="E35" s="45">
         <f>E30+E31-E32-E33-E34</f>
         <v>81</v>
       </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
       <c r="H35" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="I35" s="68" t="s">
-        <v>331</v>
-      </c>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="49">
+        <v>326</v>
+      </c>
+      <c r="I35" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="79" t="s">
+        <v>382</v>
+      </c>
+      <c r="N35" s="79"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="82"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="86" t="s">
+        <v>324</v>
+      </c>
+      <c r="E36" s="87"/>
+      <c r="F36" s="87" t="s">
+        <v>375</v>
+      </c>
+      <c r="G36" s="88"/>
+      <c r="H36" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="86" t="s">
+        <v>320</v>
+      </c>
+      <c r="K36" s="88"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="79" t="s">
+        <v>383</v>
+      </c>
+      <c r="N36" s="79"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="81"/>
+      <c r="Q36" s="82"/>
+    </row>
+    <row r="37" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="65" t="s">
+        <v>358</v>
+      </c>
+      <c r="E37" s="75"/>
+      <c r="F37" s="76" t="s">
+        <v>376</v>
+      </c>
+      <c r="G37" s="76" t="s">
+        <v>377</v>
+      </c>
+      <c r="H37" s="43" t="s">
+        <v>328</v>
+      </c>
+      <c r="I37" s="71">
         <v>0</v>
       </c>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="J37" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="K37" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="L37" s="42"/>
+      <c r="M37" s="79" t="s">
+        <v>383</v>
+      </c>
+      <c r="N37" s="79"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="81"/>
+      <c r="Q37" s="82"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="E38" s="75"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="K38" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="L38" s="42"/>
+      <c r="M38" s="79" t="s">
+        <v>384</v>
+      </c>
+      <c r="N38" s="79"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="81"/>
+      <c r="Q38" s="82"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="89"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="65" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="82" t="s">
-        <v>327</v>
-      </c>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="76" t="s">
-        <v>321</v>
-      </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
-        <v>361</v>
-      </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="74" t="s">
-        <v>362</v>
-      </c>
-      <c r="E37" s="84"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="43" t="s">
-        <v>332</v>
-      </c>
-      <c r="I37" s="73">
-        <v>0</v>
-      </c>
-      <c r="J37" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="K37" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
-        <v>361</v>
-      </c>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="74" t="s">
-        <v>363</v>
-      </c>
-      <c r="E38" s="84"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="I38" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="K38" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="42"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="78"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="74" t="s">
-        <v>364</v>
-      </c>
-      <c r="E39" s="74"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
       <c r="H39" s="43" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="J39" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="K39" s="47" t="s">
-        <v>316</v>
+      <c r="J39" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="K39" s="46" t="s">
+        <v>315</v>
       </c>
       <c r="L39" s="42"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="78"/>
-      <c r="B40" s="78"/>
+      <c r="M39" s="79" t="s">
+        <v>384</v>
+      </c>
+      <c r="N39" s="79"/>
+      <c r="O39" s="80"/>
+      <c r="P39" s="81"/>
+      <c r="Q39" s="82"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="89"/>
+      <c r="B40" s="89"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="81"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="91"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
       <c r="K40" s="42"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="79" t="s">
+      <c r="M40" s="79" t="s">
+        <v>384</v>
+      </c>
+      <c r="N40" s="79"/>
+      <c r="O40" s="80"/>
+      <c r="P40" s="81"/>
+      <c r="Q40" s="82"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="90" t="s">
+        <v>329</v>
+      </c>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="90"/>
+      <c r="I41" s="77" t="s">
+        <v>330</v>
+      </c>
+      <c r="J41" s="78"/>
+      <c r="K41" s="78"/>
+      <c r="L41" s="78"/>
+      <c r="M41" s="78"/>
+      <c r="N41" s="78"/>
+      <c r="O41" s="78"/>
+      <c r="P41" s="78"/>
+      <c r="Q41" s="78"/>
+    </row>
+    <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="C42" s="50" t="s">
+        <v>346</v>
+      </c>
+      <c r="D42" s="50" t="s">
+        <v>347</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="F42" s="50" t="s">
+        <v>349</v>
+      </c>
+      <c r="G42" s="50" t="s">
         <v>333</v>
       </c>
-      <c r="B41" s="79"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="80" t="s">
+      <c r="H42" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="J41" s="80"/>
-      <c r="K41" s="80"/>
-      <c r="L41" s="80"/>
-      <c r="M41" s="80"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="80"/>
-      <c r="P41" s="80"/>
-    </row>
-    <row r="42" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
+      <c r="I42" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="J42" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="C42" s="52" t="s">
-        <v>350</v>
-      </c>
-      <c r="D42" s="52" t="s">
-        <v>351</v>
-      </c>
-      <c r="E42" s="52" t="s">
-        <v>352</v>
-      </c>
-      <c r="F42" s="52" t="s">
-        <v>353</v>
-      </c>
-      <c r="G42" s="52" t="s">
+      <c r="K42" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="H42" s="50" t="s">
+      <c r="L42" s="49" t="s">
         <v>338</v>
       </c>
-      <c r="I42" s="51" t="s">
+      <c r="M42" s="49" t="s">
         <v>339</v>
       </c>
-      <c r="J42" s="51" t="s">
+      <c r="N42" s="49" t="s">
         <v>340</v>
       </c>
-      <c r="K42" s="51" t="s">
+      <c r="O42" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="L42" s="51" t="s">
+      <c r="P42" s="49" t="s">
         <v>342</v>
       </c>
-      <c r="M42" s="51" t="s">
+      <c r="Q42" s="56" t="s">
         <v>343</v>
       </c>
-      <c r="N42" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="O42" s="51" t="s">
-        <v>345</v>
-      </c>
-      <c r="P42" s="51" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="53">
-        <f>+IFERROR((M26/D26),0)</f>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="51">
+        <f>+IFERROR((L26/D26),0)</f>
         <v>10000</v>
       </c>
-      <c r="B43" s="54">
+      <c r="B43" s="52">
         <f>D5-A5</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="C43" s="60">
+      <c r="C43" s="58">
         <f>(HOUR(B43)*60)+(MINUTE(B43))-60</f>
         <v>660</v>
       </c>
-      <c r="D43" s="46">
+      <c r="D43" s="45">
         <f>+COUNTA(B8:B25)*60</f>
         <v>0</v>
       </c>
-      <c r="E43" s="55">
+      <c r="E43" s="53">
         <f>IFERROR(C43/D43,0)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="46">
+      <c r="F43" s="45">
         <v>5</v>
       </c>
-      <c r="G43" s="46">
+      <c r="G43" s="45">
         <v>7</v>
       </c>
-      <c r="H43" s="53">
+      <c r="H43" s="51">
         <f>IFERROR(H5/F43,0)</f>
         <v>0</v>
       </c>
-      <c r="I43" s="56">
-        <f>IFERROR(E26/$M$26,0)</f>
+      <c r="I43" s="54">
+        <f>IFERROR(E26/$L$26,0)</f>
         <v>0.26</v>
       </c>
-      <c r="J43" s="56">
-        <f>IFERROR(F26/$M$26,0)</f>
+      <c r="J43" s="54">
+        <f>IFERROR(F26/$L$26,0)</f>
         <v>0.25333333333333335</v>
       </c>
-      <c r="K43" s="56">
-        <f>IFERROR(G26/$M$26,0)</f>
+      <c r="K43" s="54">
+        <f>IFERROR(G26/$L$26,0)</f>
         <v>0.24666666666666667</v>
       </c>
-      <c r="L43" s="56">
-        <f>IFERROR(H26/$M$26,0)</f>
+      <c r="L43" s="54">
+        <f>IFERROR(H26/$L$26,0)</f>
         <v>0.24</v>
       </c>
-      <c r="M43" s="56">
-        <f>IFERROR(L33/$M$26,0)</f>
-        <v>2.2666666666666666E-4</v>
-      </c>
-      <c r="N43" s="56">
-        <f>IFERROR(I26/$M$26,0)</f>
-        <v>0.27333333333333332</v>
-      </c>
-      <c r="O43" s="56">
-        <f>IFERROR(G33/$M$26,0)</f>
+      <c r="M43" s="54">
+        <f>IFERROR(L33/$L$26,0)</f>
         <v>0</v>
       </c>
-      <c r="P43" s="56">
-        <f>IFERROR(K26/$M$26,0)</f>
+      <c r="N43" s="54">
+        <f>IFERROR(#REF!/$L$26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O43" s="54">
+        <f>IFERROR(G33/$L$26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="54">
+        <f>IFERROR(I26/$L$26,0)</f>
         <v>0.26666666666666666</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="58" t="s">
-        <v>347</v>
-      </c>
-      <c r="J44" s="58" t="s">
-        <v>348</v>
-      </c>
-      <c r="K44" s="58" t="s">
-        <v>323</v>
-      </c>
-      <c r="L44" s="58" t="s">
-        <v>349</v>
-      </c>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="56">
-        <f>IFERROR(L26/$M$26,0)</f>
+      <c r="Q43" s="54">
+        <f>IFERROR(J26/$L$26,0)</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="J45" s="56">
-        <f>IFERROR(H29/$M$26,0)</f>
+    </row>
+    <row r="44" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="55"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="56" t="s">
+        <v>344</v>
+      </c>
+      <c r="J44" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="K44" s="56" t="s">
+        <v>345</v>
+      </c>
+      <c r="M44" s="55"/>
+      <c r="N44" s="55"/>
+      <c r="O44" s="55"/>
+      <c r="P44" s="55"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="55"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="54">
+        <f>IFERROR(H29/$L$26,0)</f>
         <v>1.3333333333333333E-5</v>
       </c>
-      <c r="K45" s="59">
+      <c r="J45" s="57">
         <f>IFERROR(M30/D26,0)</f>
-        <v>300</v>
-      </c>
-      <c r="L45" s="59">
+        <v>460</v>
+      </c>
+      <c r="K45" s="57">
         <f>IFERROR(H26/D26,0)</f>
         <v>2400</v>
       </c>
       <c r="M45" s="2"/>
-      <c r="N45" s="57"/>
-      <c r="O45" s="57"/>
-      <c r="P45" s="57"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="55"/>
+      <c r="P45" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="72">
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M30:P30"/>
     <mergeCell ref="H30:I30"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="A2:C2"/>
@@ -4447,47 +4629,68 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:K6"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="L28:L29"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="M6:O6"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A41:H41"/>
-    <mergeCell ref="I41:P41"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="M28:Q28"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="M31:Q31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="I41:Q41"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{AEF5EDB9-E736-4AB4-A9AF-637FA36B9F1A}">
@@ -4526,11 +4729,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Cambio de nombre de clases y ajustes para la creacion de la bitacora conectandose con el proyecto de persistencia
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDDDA99-3EE8-4DC1-8D94-9A7E43E732CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB724F-CB37-4A3C-B054-16D48C01ADE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="388">
   <si>
     <t>Fecha</t>
   </si>
@@ -1098,9 +1098,6 @@
     <t>no se</t>
   </si>
   <si>
-    <t>26/03/2024</t>
-  </si>
-  <si>
     <t>Proveedor</t>
   </si>
   <si>
@@ -1197,7 +1194,13 @@
     <t>Cemento Kilos Pulida Dia</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>2024-03-26</t>
+  </si>
+  <si>
+    <t>Maquina 1</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1391,6 +1394,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF8EA9DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="8EA9DB"/>
       </patternFill>
     </fill>
   </fills>
@@ -1599,7 +1607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1819,170 +1827,230 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3050,210 +3118,210 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36:G39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.28515625"/>
+    <col min="2" max="2" customWidth="true" width="10.85546875"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="6" max="6" customWidth="true" width="10.140625"/>
+    <col min="7" max="7" customWidth="true" width="10.42578125"/>
+    <col min="8" max="8" customWidth="true" width="10.7109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5703125"/>
+    <col min="10" max="11" customWidth="true" width="10.5703125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625"/>
+    <col min="13" max="13" customWidth="true" width="9.140625"/>
+    <col min="14" max="14" customWidth="true" width="8.7109375"/>
+    <col min="15" max="15" customWidth="true" width="13.28515625"/>
+    <col min="16" max="16" customWidth="true" width="11.7109375"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="19.85546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="115" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="111" t="s">
+      <c r="O2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
-        <v>353</v>
-      </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="115" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="115"/>
-      <c r="F3" s="118" t="s">
+      <c r="A3" t="s" s="151">
+        <v>387</v>
+      </c>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" s="93"/>
+      <c r="F3" t="s" s="151">
         <v>20</v>
       </c>
-      <c r="G3" s="120"/>
-      <c r="H3" s="121">
-        <v>8</v>
-      </c>
-      <c r="I3" s="120"/>
-      <c r="J3" s="118" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="98" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="94"/>
+      <c r="J3" t="s" s="151">
         <v>351</v>
       </c>
-      <c r="K3" s="122"/>
-      <c r="L3" s="120"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="94"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="112" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="83" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="112" t="s">
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="83" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="112" t="s">
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="83" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="114"/>
+      <c r="M4" s="85"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="111" t="s">
+      <c r="O4" s="90" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="94">
+      <c r="A5" s="123">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="94">
+      <c r="B5" s="124"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="123">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="99"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="106"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="116">
-        <v>123</v>
-      </c>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
+      <c r="O5" t="n" s="151">
+        <v>12345.0</v>
+      </c>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="86" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="103" t="s">
+      <c r="B6" s="86"/>
+      <c r="C6" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="105" t="s">
+      <c r="D6" s="100"/>
+      <c r="E6" s="102" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="108" t="s">
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="J6" s="109"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="104" t="s">
+      <c r="J6" s="88"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="101" t="s">
         <v>299</v>
       </c>
-      <c r="M6" s="128" t="s">
+      <c r="M6" s="108" t="s">
         <v>300</v>
       </c>
-      <c r="N6" s="129"/>
-      <c r="O6" s="130"/>
-      <c r="P6" s="117" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q6" s="117"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="97" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q6" s="97"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3287,9 +3355,9 @@
         <v>298</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>364</v>
-      </c>
-      <c r="L7" s="104"/>
+        <v>363</v>
+      </c>
+      <c r="L7" s="101"/>
       <c r="M7" s="26" t="s">
         <v>301</v>
       </c>
@@ -3303,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3355,7 +3423,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="73" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3407,7 +3475,7 @@
         <v>10</v>
       </c>
       <c r="Q9" s="73" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3457,7 +3525,7 @@
         <v>12</v>
       </c>
       <c r="Q10" s="73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -3501,7 +3569,7 @@
         <v>13</v>
       </c>
       <c r="Q11" s="73" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
@@ -3545,7 +3613,7 @@
         <v>14</v>
       </c>
       <c r="Q12" s="74" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -3589,7 +3657,7 @@
         <v>15</v>
       </c>
       <c r="Q13" s="73" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3633,7 +3701,7 @@
         <v>16</v>
       </c>
       <c r="Q14" s="73" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -3677,7 +3745,7 @@
         <v>17</v>
       </c>
       <c r="Q15" s="73" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -3998,11 +4066,11 @@
       <c r="A27" s="64"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -4018,35 +4086,35 @@
         <v>2</v>
       </c>
       <c r="B28" s="43" t="s">
+        <v>353</v>
+      </c>
+      <c r="C28" s="67" t="s">
         <v>354</v>
       </c>
-      <c r="C28" s="67" t="s">
-        <v>355</v>
-      </c>
-      <c r="D28" s="100" t="s">
+      <c r="D28" s="82" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100" t="s">
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="I28" s="100"/>
-      <c r="J28" s="100" t="s">
+      <c r="I28" s="82"/>
+      <c r="J28" s="82" t="s">
         <v>319</v>
       </c>
-      <c r="K28" s="100"/>
-      <c r="L28" s="101" t="s">
-        <v>385</v>
-      </c>
-      <c r="M28" s="100" t="s">
+      <c r="K28" s="82"/>
+      <c r="L28" s="107" t="s">
+        <v>384</v>
+      </c>
+      <c r="M28" s="82" t="s">
         <v>321</v>
       </c>
-      <c r="N28" s="100"/>
-      <c r="O28" s="100"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="100"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
     </row>
     <row r="29" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -4056,32 +4124,32 @@
       <c r="C29" s="63"/>
       <c r="D29" s="59"/>
       <c r="E29" s="67" t="s">
+        <v>361</v>
+      </c>
+      <c r="F29" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="G29" s="67" t="s">
         <v>362</v>
       </c>
-      <c r="F29" s="67" t="s">
-        <v>361</v>
-      </c>
-      <c r="G29" s="67" t="s">
-        <v>363</v>
-      </c>
-      <c r="H29" s="125">
+      <c r="H29" s="80">
         <v>2</v>
       </c>
-      <c r="I29" s="126"/>
+      <c r="I29" s="81"/>
       <c r="J29" s="43" t="s">
         <v>322</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="101"/>
-      <c r="M29" s="131">
+      <c r="L29" s="107"/>
+      <c r="M29" s="119">
         <v>8</v>
       </c>
-      <c r="N29" s="131"/>
-      <c r="O29" s="131"/>
-      <c r="P29" s="131"/>
-      <c r="Q29" s="131"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
+      <c r="P29" s="119"/>
+      <c r="Q29" s="119"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
@@ -4095,14 +4163,16 @@
       <c r="E30" s="45">
         <v>116</v>
       </c>
-      <c r="F30" s="45" t="s">
-        <v>386</v>
-      </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="100" t="s">
+      <c r="F30" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s" s="151">
+        <v>20</v>
+      </c>
+      <c r="H30" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="I30" s="100"/>
+      <c r="I30" s="82"/>
       <c r="J30" s="45">
         <v>2</v>
       </c>
@@ -4110,14 +4180,14 @@
         <v>60</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="131">
+      <c r="M30" s="119">
         <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
         <v>6900</v>
       </c>
-      <c r="N30" s="131"/>
-      <c r="O30" s="131"/>
-      <c r="P30" s="131"/>
-      <c r="Q30" s="131"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
+      <c r="P30" s="119"/>
+      <c r="Q30" s="119"/>
     </row>
     <row r="31" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
@@ -4140,13 +4210,13 @@
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="42"/>
-      <c r="M31" s="84" t="s">
-        <v>378</v>
-      </c>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
-      <c r="P31" s="85"/>
-      <c r="Q31" s="85"/>
+      <c r="M31" s="120" t="s">
+        <v>377</v>
+      </c>
+      <c r="N31" s="121"/>
+      <c r="O31" s="121"/>
+      <c r="P31" s="121"/>
+      <c r="Q31" s="121"/>
     </row>
     <row r="32" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
@@ -4171,13 +4241,13 @@
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
       <c r="L32" s="42"/>
-      <c r="M32" s="79" t="s">
-        <v>379</v>
-      </c>
-      <c r="N32" s="79"/>
-      <c r="O32" s="80"/>
-      <c r="P32" s="81"/>
-      <c r="Q32" s="82"/>
+      <c r="M32" s="122" t="s">
+        <v>378</v>
+      </c>
+      <c r="N32" s="122"/>
+      <c r="O32" s="127"/>
+      <c r="P32" s="128"/>
+      <c r="Q32" s="129"/>
     </row>
     <row r="33" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
@@ -4202,13 +4272,13 @@
       <c r="J33" s="45"/>
       <c r="K33" s="45"/>
       <c r="L33" s="42"/>
-      <c r="M33" s="79" t="s">
-        <v>380</v>
-      </c>
-      <c r="N33" s="79"/>
-      <c r="O33" s="80"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="82"/>
+      <c r="M33" s="122" t="s">
+        <v>379</v>
+      </c>
+      <c r="N33" s="122"/>
+      <c r="O33" s="127"/>
+      <c r="P33" s="128"/>
+      <c r="Q33" s="129"/>
     </row>
     <row r="34" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
@@ -4222,20 +4292,20 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
-      <c r="H34" s="123" t="s">
+      <c r="H34" s="78" t="s">
         <v>325</v>
       </c>
-      <c r="I34" s="124"/>
+      <c r="I34" s="79"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="42"/>
-      <c r="M34" s="79" t="s">
-        <v>381</v>
-      </c>
-      <c r="N34" s="79"/>
-      <c r="O34" s="80"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="82"/>
+      <c r="M34" s="122" t="s">
+        <v>380</v>
+      </c>
+      <c r="N34" s="122"/>
+      <c r="O34" s="127"/>
+      <c r="P34" s="128"/>
+      <c r="Q34" s="129"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -4261,62 +4331,62 @@
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="42"/>
-      <c r="M35" s="79" t="s">
-        <v>382</v>
-      </c>
-      <c r="N35" s="79"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="82"/>
+      <c r="M35" s="122" t="s">
+        <v>381</v>
+      </c>
+      <c r="N35" s="122"/>
+      <c r="O35" s="127"/>
+      <c r="P35" s="128"/>
+      <c r="Q35" s="129"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
-      <c r="D36" s="86" t="s">
+      <c r="D36" s="116" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87" t="s">
-        <v>375</v>
-      </c>
-      <c r="G36" s="88"/>
+      <c r="E36" s="117"/>
+      <c r="F36" s="117" t="s">
+        <v>374</v>
+      </c>
+      <c r="G36" s="118"/>
       <c r="H36" s="45" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="86" t="s">
+      <c r="J36" s="116" t="s">
         <v>320</v>
       </c>
-      <c r="K36" s="88"/>
+      <c r="K36" s="118"/>
       <c r="L36" s="42"/>
-      <c r="M36" s="79" t="s">
-        <v>383</v>
-      </c>
-      <c r="N36" s="79"/>
-      <c r="O36" s="80"/>
-      <c r="P36" s="81"/>
-      <c r="Q36" s="82"/>
-    </row>
-    <row r="37" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="M36" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="N36" s="122"/>
+      <c r="O36" s="127"/>
+      <c r="P36" s="128"/>
+      <c r="Q36" s="129"/>
+    </row>
+    <row r="37" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B37" s="63"/>
       <c r="C37" s="63"/>
       <c r="D37" s="65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E37" s="75"/>
       <c r="F37" s="76" t="s">
+        <v>375</v>
+      </c>
+      <c r="G37" s="76" t="s">
         <v>376</v>
-      </c>
-      <c r="G37" s="76" t="s">
-        <v>377</v>
       </c>
       <c r="H37" s="43" t="s">
         <v>328</v>
@@ -4331,32 +4401,28 @@
         <v>315</v>
       </c>
       <c r="L37" s="42"/>
-      <c r="M37" s="79" t="s">
-        <v>383</v>
-      </c>
-      <c r="N37" s="79"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="81"/>
-      <c r="Q37" s="82"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M37" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="N37" s="122"/>
+      <c r="O37" s="127"/>
+      <c r="P37" s="128"/>
+      <c r="Q37" s="129"/>
+    </row>
+    <row r="38" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B38" s="63"/>
       <c r="C38" s="63"/>
       <c r="D38" s="65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E38" s="75"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="I38" s="65" t="s">
-        <v>8</v>
-      </c>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="133"/>
       <c r="J38" s="45" t="s">
         <v>323</v>
       </c>
@@ -4364,30 +4430,26 @@
         <v>315</v>
       </c>
       <c r="L38" s="42"/>
-      <c r="M38" s="79" t="s">
-        <v>384</v>
-      </c>
-      <c r="N38" s="79"/>
-      <c r="O38" s="80"/>
-      <c r="P38" s="81"/>
-      <c r="Q38" s="82"/>
+      <c r="M38" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="N38" s="122"/>
+      <c r="O38" s="127"/>
+      <c r="P38" s="128"/>
+      <c r="Q38" s="129"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
-      <c r="B39" s="89"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="111"/>
       <c r="C39" s="62"/>
       <c r="D39" s="65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E39" s="65"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="43" t="s">
-        <v>328</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
+      <c r="F39" s="114"/>
+      <c r="G39" s="114"/>
+      <c r="H39" s="132"/>
+      <c r="I39" s="133"/>
       <c r="J39" s="45" t="s">
         <v>323</v>
       </c>
@@ -4395,57 +4457,57 @@
         <v>315</v>
       </c>
       <c r="L39" s="42"/>
-      <c r="M39" s="79" t="s">
-        <v>384</v>
-      </c>
-      <c r="N39" s="79"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="81"/>
-      <c r="Q39" s="82"/>
+      <c r="M39" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="N39" s="122"/>
+      <c r="O39" s="127"/>
+      <c r="P39" s="128"/>
+      <c r="Q39" s="129"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="89"/>
-      <c r="B40" s="89"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="89"/>
-      <c r="E40" s="89"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="91"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="95"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
       <c r="K40" s="42"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="79" t="s">
-        <v>384</v>
-      </c>
-      <c r="N40" s="79"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="81"/>
-      <c r="Q40" s="82"/>
+      <c r="M40" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="N40" s="122"/>
+      <c r="O40" s="127"/>
+      <c r="P40" s="128"/>
+      <c r="Q40" s="129"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="112" t="s">
         <v>329</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="77" t="s">
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="130" t="s">
         <v>330</v>
       </c>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78"/>
-      <c r="L41" s="78"/>
-      <c r="M41" s="78"/>
-      <c r="N41" s="78"/>
-      <c r="O41" s="78"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="78"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="131"/>
+      <c r="M41" s="131"/>
+      <c r="N41" s="131"/>
+      <c r="O41" s="131"/>
+      <c r="P41" s="131"/>
+      <c r="Q41" s="131"/>
     </row>
     <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
@@ -4618,49 +4680,23 @@
       <c r="P45" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
+  <mergeCells count="74">
+    <mergeCell ref="I41:Q41"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O36:Q36"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="M28:Q28"/>
     <mergeCell ref="D36:E36"/>
@@ -4677,20 +4713,48 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="H5:K5"/>
-    <mergeCell ref="O32:Q32"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="I41:Q41"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{AEF5EDB9-E736-4AB4-A9AF-637FA36B9F1A}">
@@ -4705,7 +4769,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I33" xr:uid="{FB065D7C-B20C-4A8C-BBDD-59A3B275D760}">
       <formula1>"Empleado 1, Empleado2, Empleado 3, Empleado 4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H36:I36 H38:I38" xr:uid="{2BE9F060-0544-492D-BFC4-E4092DFF73D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H36:I36" xr:uid="{2BE9F060-0544-492D-BFC4-E4092DFF73D0}">
       <formula1>"Maquina 1, Maquina 2, Maquina 3, Maquina 4, Maquina 5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4723,17 +4787,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
@@ -4983,7 +5047,7 @@
       <c r="O4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" t="s" s="0">
         <v>62</v>
       </c>
       <c r="U4" s="8" t="s">
@@ -5050,7 +5114,7 @@
       <c r="O5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" t="s" s="0">
         <v>71</v>
       </c>
       <c r="U5" s="8" t="s">

</xml_diff>

<commit_message>
se implementaros metodos para la comunicación con el proyecto de persistencia.
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB724F-CB37-4A3C-B054-16D48C01ADE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AC7EB6-7C1F-43D0-8E97-52464CB597B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="389">
   <si>
     <t>Fecha</t>
   </si>
@@ -1194,13 +1194,16 @@
     <t>Cemento Kilos Pulida Dia</t>
   </si>
   <si>
-    <t>2024-03-26</t>
-  </si>
-  <si>
     <t>Maquina 1</t>
   </si>
   <si>
-    <t>2024-04-05</t>
+    <t>2024-04-08</t>
+  </si>
+  <si>
+    <t>2024-04-09</t>
+  </si>
+  <si>
+    <t>2024-04-10</t>
   </si>
 </sst>
 </file>
@@ -1607,7 +1610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,6 +1833,150 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1842,18 +1989,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1866,143 +2001,8 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -3118,8 +3118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,185 +3143,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="86" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90" t="s">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90" t="s">
+      <c r="G2" s="109"/>
+      <c r="H2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="90" t="s">
+      <c r="O2" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="151">
-        <v>387</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93" t="s">
-        <v>386</v>
-      </c>
-      <c r="E3" s="93"/>
-      <c r="F3" t="s" s="151">
+      <c r="A3" t="s" s="150">
+        <v>388</v>
+      </c>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="113" t="s">
+        <v>385</v>
+      </c>
+      <c r="E3" s="113"/>
+      <c r="F3" t="s" s="150">
         <v>20</v>
       </c>
-      <c r="G3" s="94"/>
-      <c r="H3" s="98" t="s">
+      <c r="G3" s="118"/>
+      <c r="H3" s="117" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="94"/>
-      <c r="J3" t="s" s="151">
+      <c r="I3" s="118"/>
+      <c r="J3" t="s" s="150">
         <v>351</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="94"/>
+      <c r="K3" s="119"/>
+      <c r="L3" s="118"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="110" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="83" t="s">
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="110" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="83" t="s">
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="110" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="83" t="s">
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="110" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="85"/>
+      <c r="M4" s="112"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="90" t="s">
+      <c r="O4" s="109" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="123">
+      <c r="A5" s="94">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="124"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="123">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="94">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="106"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="99"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="151">
-        <v>12345.0</v>
-      </c>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
+      <c r="O5" t="n" s="150">
+        <v>6843.0</v>
+      </c>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="130" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="100" t="s">
+      <c r="B6" s="130"/>
+      <c r="C6" s="120" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="102" t="s">
+      <c r="D6" s="120"/>
+      <c r="E6" s="122" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="87" t="s">
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="131" t="s">
         <v>296</v>
       </c>
-      <c r="J6" s="88"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="101" t="s">
+      <c r="J6" s="132"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="121" t="s">
         <v>299</v>
       </c>
-      <c r="M6" s="108" t="s">
+      <c r="M6" s="106" t="s">
         <v>300</v>
       </c>
-      <c r="N6" s="109"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="97" t="s">
+      <c r="N6" s="107"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="116" t="s">
         <v>364</v>
       </c>
-      <c r="Q6" s="97"/>
+      <c r="Q6" s="116"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3357,7 +3357,7 @@
       <c r="K7" s="36" t="s">
         <v>363</v>
       </c>
-      <c r="L7" s="101"/>
+      <c r="L7" s="121"/>
       <c r="M7" s="26" t="s">
         <v>301</v>
       </c>
@@ -4066,11 +4066,11 @@
       <c r="A27" s="64"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="102"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -4091,30 +4091,30 @@
       <c r="C28" s="67" t="s">
         <v>354</v>
       </c>
-      <c r="D28" s="82" t="s">
+      <c r="D28" s="87" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82" t="s">
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87" t="s">
         <v>313</v>
       </c>
-      <c r="I28" s="82"/>
-      <c r="J28" s="82" t="s">
+      <c r="I28" s="87"/>
+      <c r="J28" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="K28" s="82"/>
-      <c r="L28" s="107" t="s">
+      <c r="K28" s="87"/>
+      <c r="L28" s="105" t="s">
         <v>384</v>
       </c>
-      <c r="M28" s="82" t="s">
+      <c r="M28" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="N28" s="82"/>
-      <c r="O28" s="82"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="82"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="87"/>
     </row>
     <row r="29" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -4132,24 +4132,24 @@
       <c r="G29" s="67" t="s">
         <v>362</v>
       </c>
-      <c r="H29" s="80">
+      <c r="H29" s="128">
         <v>2</v>
       </c>
-      <c r="I29" s="81"/>
+      <c r="I29" s="129"/>
       <c r="J29" s="43" t="s">
         <v>322</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="107"/>
-      <c r="M29" s="119">
+      <c r="L29" s="105"/>
+      <c r="M29" s="91">
         <v>8</v>
       </c>
-      <c r="N29" s="119"/>
-      <c r="O29" s="119"/>
-      <c r="P29" s="119"/>
-      <c r="Q29" s="119"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="91"/>
+      <c r="P29" s="91"/>
+      <c r="Q29" s="91"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
@@ -4166,13 +4166,13 @@
       <c r="F30" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="G30" t="s" s="151">
+      <c r="G30" t="s" s="150">
         <v>20</v>
       </c>
-      <c r="H30" s="82" t="s">
+      <c r="H30" s="87" t="s">
         <v>314</v>
       </c>
-      <c r="I30" s="82"/>
+      <c r="I30" s="87"/>
       <c r="J30" s="45">
         <v>2</v>
       </c>
@@ -4180,14 +4180,14 @@
         <v>60</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="119">
+      <c r="M30" s="91">
         <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
         <v>6900</v>
       </c>
-      <c r="N30" s="119"/>
-      <c r="O30" s="119"/>
-      <c r="P30" s="119"/>
-      <c r="Q30" s="119"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
     </row>
     <row r="31" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
@@ -4210,13 +4210,13 @@
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="42"/>
-      <c r="M31" s="120" t="s">
+      <c r="M31" s="92" t="s">
         <v>377</v>
       </c>
-      <c r="N31" s="121"/>
-      <c r="O31" s="121"/>
-      <c r="P31" s="121"/>
-      <c r="Q31" s="121"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="93"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="93"/>
     </row>
     <row r="32" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
@@ -4241,13 +4241,13 @@
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
       <c r="L32" s="42"/>
-      <c r="M32" s="122" t="s">
+      <c r="M32" s="80" t="s">
         <v>378</v>
       </c>
-      <c r="N32" s="122"/>
-      <c r="O32" s="127"/>
-      <c r="P32" s="128"/>
-      <c r="Q32" s="129"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="81"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="83"/>
     </row>
     <row r="33" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
@@ -4272,13 +4272,13 @@
       <c r="J33" s="45"/>
       <c r="K33" s="45"/>
       <c r="L33" s="42"/>
-      <c r="M33" s="122" t="s">
+      <c r="M33" s="80" t="s">
         <v>379</v>
       </c>
-      <c r="N33" s="122"/>
-      <c r="O33" s="127"/>
-      <c r="P33" s="128"/>
-      <c r="Q33" s="129"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="81"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="83"/>
     </row>
     <row r="34" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
@@ -4292,20 +4292,20 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
-      <c r="H34" s="78" t="s">
+      <c r="H34" s="126" t="s">
         <v>325</v>
       </c>
-      <c r="I34" s="79"/>
+      <c r="I34" s="127"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="42"/>
-      <c r="M34" s="122" t="s">
+      <c r="M34" s="80" t="s">
         <v>380</v>
       </c>
-      <c r="N34" s="122"/>
-      <c r="O34" s="127"/>
-      <c r="P34" s="128"/>
-      <c r="Q34" s="129"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="82"/>
+      <c r="Q34" s="83"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -4331,13 +4331,13 @@
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="42"/>
-      <c r="M35" s="122" t="s">
+      <c r="M35" s="80" t="s">
         <v>381</v>
       </c>
-      <c r="N35" s="122"/>
-      <c r="O35" s="127"/>
-      <c r="P35" s="128"/>
-      <c r="Q35" s="129"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="82"/>
+      <c r="Q35" s="83"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
@@ -4345,32 +4345,32 @@
       </c>
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
-      <c r="D36" s="116" t="s">
+      <c r="D36" s="88" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="117"/>
-      <c r="F36" s="117" t="s">
+      <c r="E36" s="89"/>
+      <c r="F36" s="89" t="s">
         <v>374</v>
       </c>
-      <c r="G36" s="118"/>
+      <c r="G36" s="90"/>
       <c r="H36" s="45" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="116" t="s">
+      <c r="J36" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="K36" s="118"/>
+      <c r="K36" s="90"/>
       <c r="L36" s="42"/>
-      <c r="M36" s="122" t="s">
+      <c r="M36" s="80" t="s">
         <v>382</v>
       </c>
-      <c r="N36" s="122"/>
-      <c r="O36" s="127"/>
-      <c r="P36" s="128"/>
-      <c r="Q36" s="129"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="81"/>
+      <c r="P36" s="82"/>
+      <c r="Q36" s="83"/>
     </row>
     <row r="37" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
@@ -4392,7 +4392,7 @@
         <v>328</v>
       </c>
       <c r="I37" s="71">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J37" s="45" t="s">
         <v>323</v>
@@ -4401,13 +4401,13 @@
         <v>315</v>
       </c>
       <c r="L37" s="42"/>
-      <c r="M37" s="122" t="s">
+      <c r="M37" s="80" t="s">
         <v>382</v>
       </c>
-      <c r="N37" s="122"/>
-      <c r="O37" s="127"/>
-      <c r="P37" s="128"/>
-      <c r="Q37" s="129"/>
+      <c r="N37" s="80"/>
+      <c r="O37" s="81"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="83"/>
     </row>
     <row r="38" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
@@ -4419,10 +4419,10 @@
         <v>358</v>
       </c>
       <c r="E38" s="75"/>
-      <c r="F38" s="113"/>
-      <c r="G38" s="113"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="133"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="103"/>
+      <c r="H38" s="84"/>
+      <c r="I38" s="85"/>
       <c r="J38" s="45" t="s">
         <v>323</v>
       </c>
@@ -4430,26 +4430,26 @@
         <v>315</v>
       </c>
       <c r="L38" s="42"/>
-      <c r="M38" s="122" t="s">
+      <c r="M38" s="80" t="s">
         <v>383</v>
       </c>
-      <c r="N38" s="122"/>
-      <c r="O38" s="127"/>
-      <c r="P38" s="128"/>
-      <c r="Q38" s="129"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="81"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="83"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
-      <c r="B39" s="111"/>
+      <c r="A39" s="100"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="62"/>
       <c r="D39" s="65" t="s">
         <v>359</v>
       </c>
       <c r="E39" s="65"/>
-      <c r="F39" s="114"/>
-      <c r="G39" s="114"/>
-      <c r="H39" s="132"/>
-      <c r="I39" s="133"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="104"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="85"/>
       <c r="J39" s="45" t="s">
         <v>323</v>
       </c>
@@ -4457,57 +4457,57 @@
         <v>315</v>
       </c>
       <c r="L39" s="42"/>
-      <c r="M39" s="122" t="s">
+      <c r="M39" s="80" t="s">
         <v>383</v>
       </c>
-      <c r="N39" s="122"/>
-      <c r="O39" s="127"/>
-      <c r="P39" s="128"/>
-      <c r="Q39" s="129"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="81"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="83"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="111"/>
-      <c r="B40" s="111"/>
+      <c r="A40" s="100"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="95"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="102"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
       <c r="K40" s="42"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="122" t="s">
+      <c r="M40" s="80" t="s">
         <v>383</v>
       </c>
-      <c r="N40" s="122"/>
-      <c r="O40" s="127"/>
-      <c r="P40" s="128"/>
-      <c r="Q40" s="129"/>
+      <c r="N40" s="80"/>
+      <c r="O40" s="81"/>
+      <c r="P40" s="82"/>
+      <c r="Q40" s="83"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="112" t="s">
+      <c r="A41" s="101" t="s">
         <v>329</v>
       </c>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112"/>
-      <c r="H41" s="112"/>
-      <c r="I41" s="130" t="s">
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="101"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="J41" s="131"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="131"/>
-      <c r="M41" s="131"/>
-      <c r="N41" s="131"/>
-      <c r="O41" s="131"/>
-      <c r="P41" s="131"/>
-      <c r="Q41" s="131"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="79"/>
+      <c r="O41" s="79"/>
+      <c r="P41" s="79"/>
+      <c r="Q41" s="79"/>
     </row>
     <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
@@ -4681,22 +4681,48 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="I41:Q41"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="O32:Q32"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="M28:Q28"/>
     <mergeCell ref="D36:E36"/>
@@ -4713,48 +4739,22 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="I41:Q41"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{AEF5EDB9-E736-4AB4-A9AF-637FA36B9F1A}">

</xml_diff>

<commit_message>
Metodos para enviar datos para el proyecto de persistencia.
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AC7EB6-7C1F-43D0-8E97-52464CB597B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F8E3A-9A45-4930-B9D9-48101D298EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="387">
   <si>
     <t>Fecha</t>
   </si>
@@ -1197,13 +1197,7 @@
     <t>Maquina 1</t>
   </si>
   <si>
-    <t>2024-04-08</t>
-  </si>
-  <si>
-    <t>2024-04-09</t>
-  </si>
-  <si>
-    <t>2024-04-10</t>
+    <t>2024-04-14</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1830,215 +1824,176 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -3118,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,185 +3098,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="114" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109" t="s">
+      <c r="E2" s="89"/>
+      <c r="F2" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109" t="s">
+      <c r="G2" s="89"/>
+      <c r="H2" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109" t="s">
+      <c r="I2" s="89"/>
+      <c r="J2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="109" t="s">
+      <c r="O2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="150">
-        <v>388</v>
-      </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="113" t="s">
+      <c r="A3" t="s" s="137">
+        <v>386</v>
+      </c>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92" t="s">
         <v>385</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" t="s" s="150">
+      <c r="E3" s="92"/>
+      <c r="F3" t="s" s="137">
         <v>20</v>
       </c>
-      <c r="G3" s="118"/>
-      <c r="H3" s="117" t="s">
+      <c r="G3" s="93"/>
+      <c r="H3" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="118"/>
-      <c r="J3" t="s" s="150">
+      <c r="I3" s="93"/>
+      <c r="J3" t="s" s="137">
         <v>351</v>
       </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="118"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="93"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="113"/>
-      <c r="Q3" s="113"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="110" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="82" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="110" t="s">
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="82" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="110" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="82" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="112"/>
+      <c r="M4" s="84"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="109" t="s">
+      <c r="O4" s="89" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="109"/>
-      <c r="Q4" s="109"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="94">
+      <c r="A5" s="122">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="94">
+      <c r="B5" s="123"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="122">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="99"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="105"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="150">
-        <v>6843.0</v>
-      </c>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
+      <c r="O5" t="n" s="137">
+        <v>3627.0</v>
+      </c>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="130" t="s">
+      <c r="A6" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="130"/>
-      <c r="C6" s="120" t="s">
+      <c r="B6" s="85"/>
+      <c r="C6" s="99" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="120"/>
-      <c r="E6" s="122" t="s">
+      <c r="D6" s="99"/>
+      <c r="E6" s="101" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="131" t="s">
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="J6" s="132"/>
-      <c r="K6" s="133"/>
-      <c r="L6" s="121" t="s">
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="M6" s="106" t="s">
+      <c r="M6" s="107" t="s">
         <v>300</v>
       </c>
-      <c r="N6" s="107"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="116" t="s">
+      <c r="N6" s="108"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="Q6" s="116"/>
+      <c r="Q6" s="96"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3357,7 +3312,7 @@
       <c r="K7" s="36" t="s">
         <v>363</v>
       </c>
-      <c r="L7" s="121"/>
+      <c r="L7" s="100"/>
       <c r="M7" s="26" t="s">
         <v>301</v>
       </c>
@@ -4066,11 +4021,11 @@
       <c r="A27" s="64"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="102"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -4091,30 +4046,30 @@
       <c r="C28" s="67" t="s">
         <v>354</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87" t="s">
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81" t="s">
         <v>313</v>
       </c>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87" t="s">
+      <c r="I28" s="81"/>
+      <c r="J28" s="81" t="s">
         <v>319</v>
       </c>
-      <c r="K28" s="87"/>
-      <c r="L28" s="105" t="s">
+      <c r="K28" s="81"/>
+      <c r="L28" s="106" t="s">
         <v>384</v>
       </c>
-      <c r="M28" s="87" t="s">
+      <c r="M28" s="81" t="s">
         <v>321</v>
       </c>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
-      <c r="P28" s="87"/>
-      <c r="Q28" s="87"/>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="81"/>
     </row>
     <row r="29" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -4132,24 +4087,24 @@
       <c r="G29" s="67" t="s">
         <v>362</v>
       </c>
-      <c r="H29" s="128">
+      <c r="H29" s="79">
         <v>2</v>
       </c>
-      <c r="I29" s="129"/>
+      <c r="I29" s="80"/>
       <c r="J29" s="43" t="s">
         <v>322</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="105"/>
-      <c r="M29" s="91">
+      <c r="L29" s="106"/>
+      <c r="M29" s="118">
         <v>8</v>
       </c>
-      <c r="N29" s="91"/>
-      <c r="O29" s="91"/>
-      <c r="P29" s="91"/>
-      <c r="Q29" s="91"/>
+      <c r="N29" s="118"/>
+      <c r="O29" s="118"/>
+      <c r="P29" s="118"/>
+      <c r="Q29" s="118"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
@@ -4163,16 +4118,14 @@
       <c r="E30" s="45">
         <v>116</v>
       </c>
-      <c r="F30" s="77" t="s">
+      <c r="F30" s="45"/>
+      <c r="G30" t="s" s="137">
         <v>20</v>
       </c>
-      <c r="G30" t="s" s="150">
-        <v>20</v>
-      </c>
-      <c r="H30" s="87" t="s">
+      <c r="H30" s="81" t="s">
         <v>314</v>
       </c>
-      <c r="I30" s="87"/>
+      <c r="I30" s="81"/>
       <c r="J30" s="45">
         <v>2</v>
       </c>
@@ -4180,14 +4133,14 @@
         <v>60</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="91">
+      <c r="M30" s="118">
         <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
         <v>6900</v>
       </c>
-      <c r="N30" s="91"/>
-      <c r="O30" s="91"/>
-      <c r="P30" s="91"/>
-      <c r="Q30" s="91"/>
+      <c r="N30" s="118"/>
+      <c r="O30" s="118"/>
+      <c r="P30" s="118"/>
+      <c r="Q30" s="118"/>
     </row>
     <row r="31" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
@@ -4210,13 +4163,13 @@
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="42"/>
-      <c r="M31" s="92" t="s">
+      <c r="M31" s="119" t="s">
         <v>377</v>
       </c>
-      <c r="N31" s="93"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="93"/>
-      <c r="Q31" s="93"/>
+      <c r="N31" s="120"/>
+      <c r="O31" s="120"/>
+      <c r="P31" s="120"/>
+      <c r="Q31" s="120"/>
     </row>
     <row r="32" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
@@ -4241,13 +4194,13 @@
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
       <c r="L32" s="42"/>
-      <c r="M32" s="80" t="s">
+      <c r="M32" s="121" t="s">
         <v>378</v>
       </c>
-      <c r="N32" s="80"/>
-      <c r="O32" s="81"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="83"/>
+      <c r="N32" s="121"/>
+      <c r="O32" s="126"/>
+      <c r="P32" s="127"/>
+      <c r="Q32" s="128"/>
     </row>
     <row r="33" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
@@ -4272,13 +4225,13 @@
       <c r="J33" s="45"/>
       <c r="K33" s="45"/>
       <c r="L33" s="42"/>
-      <c r="M33" s="80" t="s">
+      <c r="M33" s="121" t="s">
         <v>379</v>
       </c>
-      <c r="N33" s="80"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="83"/>
+      <c r="N33" s="121"/>
+      <c r="O33" s="126"/>
+      <c r="P33" s="127"/>
+      <c r="Q33" s="128"/>
     </row>
     <row r="34" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
@@ -4292,20 +4245,20 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
-      <c r="H34" s="126" t="s">
+      <c r="H34" s="77" t="s">
         <v>325</v>
       </c>
-      <c r="I34" s="127"/>
+      <c r="I34" s="78"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="42"/>
-      <c r="M34" s="80" t="s">
+      <c r="M34" s="121" t="s">
         <v>380</v>
       </c>
-      <c r="N34" s="80"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="82"/>
-      <c r="Q34" s="83"/>
+      <c r="N34" s="121"/>
+      <c r="O34" s="126"/>
+      <c r="P34" s="127"/>
+      <c r="Q34" s="128"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -4331,13 +4284,13 @@
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="42"/>
-      <c r="M35" s="80" t="s">
+      <c r="M35" s="121" t="s">
         <v>381</v>
       </c>
-      <c r="N35" s="80"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="82"/>
-      <c r="Q35" s="83"/>
+      <c r="N35" s="121"/>
+      <c r="O35" s="126"/>
+      <c r="P35" s="127"/>
+      <c r="Q35" s="128"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
@@ -4345,32 +4298,32 @@
       </c>
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
-      <c r="D36" s="88" t="s">
+      <c r="D36" s="115" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89" t="s">
+      <c r="E36" s="116"/>
+      <c r="F36" s="116" t="s">
         <v>374</v>
       </c>
-      <c r="G36" s="90"/>
+      <c r="G36" s="117"/>
       <c r="H36" s="45" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="88" t="s">
+      <c r="J36" s="115" t="s">
         <v>320</v>
       </c>
-      <c r="K36" s="90"/>
+      <c r="K36" s="117"/>
       <c r="L36" s="42"/>
-      <c r="M36" s="80" t="s">
+      <c r="M36" s="121" t="s">
         <v>382</v>
       </c>
-      <c r="N36" s="80"/>
-      <c r="O36" s="81"/>
-      <c r="P36" s="82"/>
-      <c r="Q36" s="83"/>
+      <c r="N36" s="121"/>
+      <c r="O36" s="126"/>
+      <c r="P36" s="127"/>
+      <c r="Q36" s="128"/>
     </row>
     <row r="37" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
@@ -4401,13 +4354,13 @@
         <v>315</v>
       </c>
       <c r="L37" s="42"/>
-      <c r="M37" s="80" t="s">
+      <c r="M37" s="121" t="s">
         <v>382</v>
       </c>
-      <c r="N37" s="80"/>
-      <c r="O37" s="81"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="83"/>
+      <c r="N37" s="121"/>
+      <c r="O37" s="126"/>
+      <c r="P37" s="127"/>
+      <c r="Q37" s="128"/>
     </row>
     <row r="38" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
@@ -4419,10 +4372,14 @@
         <v>358</v>
       </c>
       <c r="E38" s="75"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="84"/>
-      <c r="I38" s="85"/>
+      <c r="F38" s="112">
+        <v>53453</v>
+      </c>
+      <c r="G38" s="112">
+        <v>45576</v>
+      </c>
+      <c r="H38" s="131"/>
+      <c r="I38" s="132"/>
       <c r="J38" s="45" t="s">
         <v>323</v>
       </c>
@@ -4430,26 +4387,26 @@
         <v>315</v>
       </c>
       <c r="L38" s="42"/>
-      <c r="M38" s="80" t="s">
+      <c r="M38" s="121" t="s">
         <v>383</v>
       </c>
-      <c r="N38" s="80"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="83"/>
+      <c r="N38" s="121"/>
+      <c r="O38" s="126"/>
+      <c r="P38" s="127"/>
+      <c r="Q38" s="128"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="100"/>
-      <c r="B39" s="100"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="62"/>
       <c r="D39" s="65" t="s">
         <v>359</v>
       </c>
       <c r="E39" s="65"/>
-      <c r="F39" s="104"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="84"/>
-      <c r="I39" s="85"/>
+      <c r="F39" s="113"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="131"/>
+      <c r="I39" s="132"/>
       <c r="J39" s="45" t="s">
         <v>323</v>
       </c>
@@ -4457,57 +4414,57 @@
         <v>315</v>
       </c>
       <c r="L39" s="42"/>
-      <c r="M39" s="80" t="s">
+      <c r="M39" s="121" t="s">
         <v>383</v>
       </c>
-      <c r="N39" s="80"/>
-      <c r="O39" s="81"/>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="83"/>
+      <c r="N39" s="121"/>
+      <c r="O39" s="126"/>
+      <c r="P39" s="127"/>
+      <c r="Q39" s="128"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="100"/>
-      <c r="B40" s="100"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
+      <c r="D40" s="110"/>
+      <c r="E40" s="110"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="102"/>
+      <c r="G40" s="110"/>
+      <c r="H40" s="94"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
       <c r="K40" s="42"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="80" t="s">
+      <c r="M40" s="121" t="s">
         <v>383</v>
       </c>
-      <c r="N40" s="80"/>
-      <c r="O40" s="81"/>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="83"/>
+      <c r="N40" s="121"/>
+      <c r="O40" s="126"/>
+      <c r="P40" s="127"/>
+      <c r="Q40" s="128"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="111" t="s">
         <v>329</v>
       </c>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="101"/>
-      <c r="F41" s="101"/>
-      <c r="G41" s="101"/>
-      <c r="H41" s="101"/>
-      <c r="I41" s="78" t="s">
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="111"/>
+      <c r="I41" s="129" t="s">
         <v>330</v>
       </c>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
-      <c r="N41" s="79"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="79"/>
-      <c r="Q41" s="79"/>
+      <c r="J41" s="130"/>
+      <c r="K41" s="130"/>
+      <c r="L41" s="130"/>
+      <c r="M41" s="130"/>
+      <c r="N41" s="130"/>
+      <c r="O41" s="130"/>
+      <c r="P41" s="130"/>
+      <c r="Q41" s="130"/>
     </row>
     <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
@@ -4681,19 +4638,51 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I41:Q41"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="M28:Q28"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="M31:Q31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M6:O6"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="G27:H27"/>
@@ -4710,51 +4699,19 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="M28:Q28"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="M29:Q29"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="M31:Q31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="O32:Q32"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="I41:Q41"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{AEF5EDB9-E736-4AB4-A9AF-637FA36B9F1A}">
@@ -4793,11 +4750,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Configuracion de errores de la aplicacion
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="390">
   <si>
     <t>Fecha</t>
   </si>
@@ -1198,6 +1198,15 @@
   </si>
   <si>
     <t>2024-04-14</t>
+  </si>
+  <si>
+    <t>2024-04-17</t>
+  </si>
+  <si>
+    <t>2024-04-19</t>
+  </si>
+  <si>
+    <t>2024-04-20</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1994,6 +2003,96 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -3157,8 +3256,8 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="137">
-        <v>386</v>
+      <c r="A3" t="s" s="167">
+        <v>389</v>
       </c>
       <c r="B3" s="91"/>
       <c r="C3" s="91"/>
@@ -3166,7 +3265,7 @@
         <v>385</v>
       </c>
       <c r="E3" s="92"/>
-      <c r="F3" t="s" s="137">
+      <c r="F3" t="s" s="167">
         <v>20</v>
       </c>
       <c r="G3" s="93"/>
@@ -3174,7 +3273,7 @@
         <v>108</v>
       </c>
       <c r="I3" s="93"/>
-      <c r="J3" t="s" s="137">
+      <c r="J3" t="s" s="167">
         <v>351</v>
       </c>
       <c r="K3" s="98"/>
@@ -3239,8 +3338,8 @@
       <c r="L5" s="104"/>
       <c r="M5" s="105"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="137">
-        <v>3627.0</v>
+      <c r="O5" t="n" s="167">
+        <v>325.0</v>
       </c>
       <c r="P5" s="95"/>
       <c r="Q5" s="95"/>
@@ -4119,7 +4218,7 @@
         <v>116</v>
       </c>
       <c r="F30" s="45"/>
-      <c r="G30" t="s" s="137">
+      <c r="G30" t="s" s="167">
         <v>20</v>
       </c>
       <c r="H30" s="81" t="s">

</xml_diff>

<commit_message>
Se agrea el plugin de History y la clase para agregar CodigoMP
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jdnar\Documents\Tesis\Aplicacion\ProcessEngine\src\main\java\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F8E3A-9A45-4930-B9D9-48101D298EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6086C50-7E17-48E0-9AC4-37B8B81ED261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plantilla" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="389">
   <si>
     <t>Fecha</t>
   </si>
@@ -1095,9 +1095,6 @@
     <t>aux1</t>
   </si>
   <si>
-    <t>no se</t>
-  </si>
-  <si>
     <t>Proveedor</t>
   </si>
   <si>
@@ -1197,16 +1194,16 @@
     <t>Maquina 1</t>
   </si>
   <si>
-    <t>2024-04-14</t>
-  </si>
-  <si>
-    <t>2024-04-17</t>
-  </si>
-  <si>
-    <t>2024-04-19</t>
-  </si>
-  <si>
-    <t>2024-04-20</t>
+    <t>2024-04-21</t>
+  </si>
+  <si>
+    <t>No se</t>
+  </si>
+  <si>
+    <t>2024-04-22</t>
+  </si>
+  <si>
+    <t>2024-04-23</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1833,6 +1830,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2003,78 +2003,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -3172,8 +3100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,185 +3125,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="115" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="89" t="s">
+      <c r="O2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
       <c r="R2" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="167">
-        <v>389</v>
-      </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="92" t="s">
-        <v>385</v>
-      </c>
-      <c r="E3" s="92"/>
-      <c r="F3" t="s" s="167">
+      <c r="A3" t="s" s="144">
+        <v>388</v>
+      </c>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93" t="s">
+        <v>384</v>
+      </c>
+      <c r="E3" s="93"/>
+      <c r="F3" t="s" s="144">
         <v>20</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="93"/>
-      <c r="J3" t="s" s="167">
+      <c r="I3" s="94"/>
+      <c r="J3" t="s" s="144">
         <v>351</v>
       </c>
-      <c r="K3" s="98"/>
-      <c r="L3" s="93"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="94"/>
       <c r="M3" s="3" t="str">
         <f>+IF(EXACT(F3,"Tuberia"),"TC","PC")</f>
         <v>TC</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
       <c r="R3" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="82" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="83" t="s">
         <v>260</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="82" t="s">
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="83" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="82" t="s">
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="83" t="s">
         <v>262</v>
       </c>
-      <c r="M4" s="84"/>
+      <c r="M4" s="85"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="89" t="s">
+      <c r="O4" s="90" t="s">
         <v>263</v>
       </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="122">
+      <c r="A5" s="123">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="122">
+      <c r="B5" s="124"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="123">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="106"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="167">
-        <v>325.0</v>
-      </c>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="95"/>
+      <c r="O5" t="n" s="144">
+        <v>123456.0</v>
+      </c>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="86" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="99" t="s">
+      <c r="B6" s="86"/>
+      <c r="C6" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" s="101" t="s">
+      <c r="D6" s="100"/>
+      <c r="E6" s="102" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="86" t="s">
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="J6" s="87"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="100" t="s">
+      <c r="J6" s="88"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="101" t="s">
         <v>299</v>
       </c>
-      <c r="M6" s="107" t="s">
+      <c r="M6" s="108" t="s">
         <v>300</v>
       </c>
-      <c r="N6" s="108"/>
-      <c r="O6" s="109"/>
-      <c r="P6" s="96" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q6" s="96"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="97" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q6" s="97"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3409,9 +3337,9 @@
         <v>298</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>363</v>
-      </c>
-      <c r="L7" s="100"/>
+        <v>362</v>
+      </c>
+      <c r="L7" s="101"/>
       <c r="M7" s="26" t="s">
         <v>301</v>
       </c>
@@ -3425,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3468,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="29" t="s">
-        <v>352</v>
+        <v>386</v>
       </c>
       <c r="O8" s="29">
         <v>1</v>
@@ -3477,7 +3405,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3520,7 +3448,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>352</v>
+        <v>386</v>
       </c>
       <c r="O9" s="29">
         <v>1</v>
@@ -3529,7 +3457,7 @@
         <v>10</v>
       </c>
       <c r="Q9" s="73" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3570,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="29" t="s">
-        <v>352</v>
+        <v>386</v>
       </c>
       <c r="O10" s="29">
         <v>1</v>
@@ -3579,7 +3507,7 @@
         <v>12</v>
       </c>
       <c r="Q10" s="73" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -3623,7 +3551,7 @@
         <v>13</v>
       </c>
       <c r="Q11" s="73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
@@ -3667,7 +3595,7 @@
         <v>14</v>
       </c>
       <c r="Q12" s="74" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -3711,7 +3639,7 @@
         <v>15</v>
       </c>
       <c r="Q13" s="73" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3755,7 +3683,7 @@
         <v>16</v>
       </c>
       <c r="Q14" s="73" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -3799,7 +3727,7 @@
         <v>17</v>
       </c>
       <c r="Q15" s="73" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4120,11 +4048,11 @@
       <c r="A27" s="64"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
@@ -4140,35 +4068,35 @@
         <v>2</v>
       </c>
       <c r="B28" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="C28" s="67" t="s">
         <v>353</v>
       </c>
-      <c r="C28" s="67" t="s">
-        <v>354</v>
-      </c>
-      <c r="D28" s="81" t="s">
+      <c r="D28" s="82" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81" t="s">
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81" t="s">
+      <c r="I28" s="82"/>
+      <c r="J28" s="82" t="s">
         <v>319</v>
       </c>
-      <c r="K28" s="81"/>
-      <c r="L28" s="106" t="s">
-        <v>384</v>
-      </c>
-      <c r="M28" s="81" t="s">
+      <c r="K28" s="82"/>
+      <c r="L28" s="107" t="s">
+        <v>383</v>
+      </c>
+      <c r="M28" s="82" t="s">
         <v>321</v>
       </c>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="81"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
     </row>
     <row r="29" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -4178,32 +4106,32 @@
       <c r="C29" s="63"/>
       <c r="D29" s="59"/>
       <c r="E29" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="F29" s="67" t="s">
+        <v>359</v>
+      </c>
+      <c r="G29" s="67" t="s">
         <v>361</v>
       </c>
-      <c r="F29" s="67" t="s">
-        <v>360</v>
-      </c>
-      <c r="G29" s="67" t="s">
-        <v>362</v>
-      </c>
-      <c r="H29" s="79">
+      <c r="H29" s="80">
         <v>2</v>
       </c>
-      <c r="I29" s="80"/>
+      <c r="I29" s="81"/>
       <c r="J29" s="43" t="s">
         <v>322</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="L29" s="106"/>
-      <c r="M29" s="118">
+      <c r="L29" s="107"/>
+      <c r="M29" s="119">
         <v>8</v>
       </c>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="118"/>
-      <c r="Q29" s="118"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
+      <c r="P29" s="119"/>
+      <c r="Q29" s="119"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
@@ -4218,13 +4146,13 @@
         <v>116</v>
       </c>
       <c r="F30" s="45"/>
-      <c r="G30" t="s" s="167">
+      <c r="G30" t="s" s="144">
         <v>20</v>
       </c>
-      <c r="H30" s="81" t="s">
+      <c r="H30" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="I30" s="81"/>
+      <c r="I30" s="82"/>
       <c r="J30" s="45">
         <v>2</v>
       </c>
@@ -4232,14 +4160,14 @@
         <v>60</v>
       </c>
       <c r="L30" s="47"/>
-      <c r="M30" s="118">
+      <c r="M30" s="119">
         <f>IF(M29=0,0,((M29*1000)/1.25)+500)</f>
         <v>6900</v>
       </c>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="118"/>
-      <c r="Q30" s="118"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
+      <c r="P30" s="119"/>
+      <c r="Q30" s="119"/>
     </row>
     <row r="31" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
@@ -4262,13 +4190,13 @@
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="42"/>
-      <c r="M31" s="119" t="s">
-        <v>377</v>
-      </c>
-      <c r="N31" s="120"/>
-      <c r="O31" s="120"/>
-      <c r="P31" s="120"/>
-      <c r="Q31" s="120"/>
+      <c r="M31" s="120" t="s">
+        <v>376</v>
+      </c>
+      <c r="N31" s="121"/>
+      <c r="O31" s="121"/>
+      <c r="P31" s="121"/>
+      <c r="Q31" s="121"/>
     </row>
     <row r="32" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
@@ -4293,13 +4221,13 @@
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
       <c r="L32" s="42"/>
-      <c r="M32" s="121" t="s">
-        <v>378</v>
-      </c>
-      <c r="N32" s="121"/>
-      <c r="O32" s="126"/>
-      <c r="P32" s="127"/>
-      <c r="Q32" s="128"/>
+      <c r="M32" s="122" t="s">
+        <v>377</v>
+      </c>
+      <c r="N32" s="122"/>
+      <c r="O32" s="127"/>
+      <c r="P32" s="128"/>
+      <c r="Q32" s="129"/>
     </row>
     <row r="33" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
@@ -4324,13 +4252,13 @@
       <c r="J33" s="45"/>
       <c r="K33" s="45"/>
       <c r="L33" s="42"/>
-      <c r="M33" s="121" t="s">
-        <v>379</v>
-      </c>
-      <c r="N33" s="121"/>
-      <c r="O33" s="126"/>
-      <c r="P33" s="127"/>
-      <c r="Q33" s="128"/>
+      <c r="M33" s="122" t="s">
+        <v>378</v>
+      </c>
+      <c r="N33" s="122"/>
+      <c r="O33" s="127"/>
+      <c r="P33" s="128"/>
+      <c r="Q33" s="129"/>
     </row>
     <row r="34" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
@@ -4344,20 +4272,20 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
-      <c r="H34" s="77" t="s">
+      <c r="H34" s="78" t="s">
         <v>325</v>
       </c>
-      <c r="I34" s="78"/>
+      <c r="I34" s="79"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="42"/>
-      <c r="M34" s="121" t="s">
-        <v>380</v>
-      </c>
-      <c r="N34" s="121"/>
-      <c r="O34" s="126"/>
-      <c r="P34" s="127"/>
-      <c r="Q34" s="128"/>
+      <c r="M34" s="122" t="s">
+        <v>379</v>
+      </c>
+      <c r="N34" s="122"/>
+      <c r="O34" s="127"/>
+      <c r="P34" s="128"/>
+      <c r="Q34" s="129"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -4383,62 +4311,62 @@
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="42"/>
-      <c r="M35" s="121" t="s">
-        <v>381</v>
-      </c>
-      <c r="N35" s="121"/>
-      <c r="O35" s="126"/>
-      <c r="P35" s="127"/>
-      <c r="Q35" s="128"/>
+      <c r="M35" s="122" t="s">
+        <v>380</v>
+      </c>
+      <c r="N35" s="122"/>
+      <c r="O35" s="127"/>
+      <c r="P35" s="128"/>
+      <c r="Q35" s="129"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
-      <c r="D36" s="115" t="s">
+      <c r="D36" s="116" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="116"/>
-      <c r="F36" s="116" t="s">
-        <v>374</v>
-      </c>
-      <c r="G36" s="117"/>
+      <c r="E36" s="117"/>
+      <c r="F36" s="117" t="s">
+        <v>373</v>
+      </c>
+      <c r="G36" s="118"/>
       <c r="H36" s="45" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="115" t="s">
+      <c r="J36" s="116" t="s">
         <v>320</v>
       </c>
-      <c r="K36" s="117"/>
+      <c r="K36" s="118"/>
       <c r="L36" s="42"/>
-      <c r="M36" s="121" t="s">
-        <v>382</v>
-      </c>
-      <c r="N36" s="121"/>
-      <c r="O36" s="126"/>
-      <c r="P36" s="127"/>
-      <c r="Q36" s="128"/>
+      <c r="M36" s="122" t="s">
+        <v>381</v>
+      </c>
+      <c r="N36" s="122"/>
+      <c r="O36" s="127"/>
+      <c r="P36" s="128"/>
+      <c r="Q36" s="129"/>
     </row>
     <row r="37" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B37" s="63"/>
       <c r="C37" s="63"/>
       <c r="D37" s="65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E37" s="75"/>
       <c r="F37" s="76" t="s">
+        <v>374</v>
+      </c>
+      <c r="G37" s="76" t="s">
         <v>375</v>
-      </c>
-      <c r="G37" s="76" t="s">
-        <v>376</v>
       </c>
       <c r="H37" s="43" t="s">
         <v>328</v>
@@ -4453,32 +4381,32 @@
         <v>315</v>
       </c>
       <c r="L37" s="42"/>
-      <c r="M37" s="121" t="s">
-        <v>382</v>
-      </c>
-      <c r="N37" s="121"/>
-      <c r="O37" s="126"/>
-      <c r="P37" s="127"/>
-      <c r="Q37" s="128"/>
+      <c r="M37" s="122" t="s">
+        <v>381</v>
+      </c>
+      <c r="N37" s="122"/>
+      <c r="O37" s="127"/>
+      <c r="P37" s="128"/>
+      <c r="Q37" s="129"/>
     </row>
     <row r="38" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" s="63"/>
       <c r="C38" s="63"/>
       <c r="D38" s="65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E38" s="75"/>
-      <c r="F38" s="112">
+      <c r="F38" s="113">
         <v>53453</v>
       </c>
-      <c r="G38" s="112">
+      <c r="G38" s="113">
         <v>45576</v>
       </c>
-      <c r="H38" s="131"/>
-      <c r="I38" s="132"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="133"/>
       <c r="J38" s="45" t="s">
         <v>323</v>
       </c>
@@ -4486,26 +4414,26 @@
         <v>315</v>
       </c>
       <c r="L38" s="42"/>
-      <c r="M38" s="121" t="s">
-        <v>383</v>
-      </c>
-      <c r="N38" s="121"/>
-      <c r="O38" s="126"/>
-      <c r="P38" s="127"/>
-      <c r="Q38" s="128"/>
+      <c r="M38" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="N38" s="122"/>
+      <c r="O38" s="127"/>
+      <c r="P38" s="128"/>
+      <c r="Q38" s="129"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="110"/>
-      <c r="B39" s="110"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="111"/>
       <c r="C39" s="62"/>
       <c r="D39" s="65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E39" s="65"/>
-      <c r="F39" s="113"/>
-      <c r="G39" s="113"/>
-      <c r="H39" s="131"/>
-      <c r="I39" s="132"/>
+      <c r="F39" s="114"/>
+      <c r="G39" s="114"/>
+      <c r="H39" s="132"/>
+      <c r="I39" s="133"/>
       <c r="J39" s="45" t="s">
         <v>323</v>
       </c>
@@ -4513,57 +4441,57 @@
         <v>315</v>
       </c>
       <c r="L39" s="42"/>
-      <c r="M39" s="121" t="s">
-        <v>383</v>
-      </c>
-      <c r="N39" s="121"/>
-      <c r="O39" s="126"/>
-      <c r="P39" s="127"/>
-      <c r="Q39" s="128"/>
+      <c r="M39" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="N39" s="122"/>
+      <c r="O39" s="127"/>
+      <c r="P39" s="128"/>
+      <c r="Q39" s="129"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="110"/>
-      <c r="B40" s="110"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="110"/>
-      <c r="H40" s="94"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="95"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
       <c r="K40" s="42"/>
       <c r="L40" s="42"/>
-      <c r="M40" s="121" t="s">
-        <v>383</v>
-      </c>
-      <c r="N40" s="121"/>
-      <c r="O40" s="126"/>
-      <c r="P40" s="127"/>
-      <c r="Q40" s="128"/>
+      <c r="M40" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="N40" s="122"/>
+      <c r="O40" s="127"/>
+      <c r="P40" s="128"/>
+      <c r="Q40" s="129"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="112" t="s">
         <v>329</v>
       </c>
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="111"/>
-      <c r="I41" s="129" t="s">
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="130" t="s">
         <v>330</v>
       </c>
-      <c r="J41" s="130"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="130"/>
-      <c r="M41" s="130"/>
-      <c r="N41" s="130"/>
-      <c r="O41" s="130"/>
-      <c r="P41" s="130"/>
-      <c r="Q41" s="130"/>
+      <c r="J41" s="131"/>
+      <c r="K41" s="131"/>
+      <c r="L41" s="131"/>
+      <c r="M41" s="131"/>
+      <c r="N41" s="131"/>
+      <c r="O41" s="131"/>
+      <c r="P41" s="131"/>
+      <c r="Q41" s="131"/>
     </row>
     <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
@@ -4849,11 +4777,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Cambios en clases para enviar el numero de bitacora
</commit_message>
<xml_diff>
--- a/src/main/java/templates/PlantillaConcreto.xlsx
+++ b/src/main/java/templates/PlantillaConcreto.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="393">
   <si>
     <t>Fecha</t>
   </si>
@@ -1204,6 +1204,18 @@
   </si>
   <si>
     <t>2024-04-23</t>
+  </si>
+  <si>
+    <t>2024-05-10</t>
+  </si>
+  <si>
+    <t>2024-05-11</t>
+  </si>
+  <si>
+    <t>2024-05-17</t>
+  </si>
+  <si>
+    <t>2024-05-16</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2003,6 +2015,69 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -3184,8 +3259,8 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="144">
-        <v>388</v>
+      <c r="A3" t="s" s="165">
+        <v>392</v>
       </c>
       <c r="B3" s="92"/>
       <c r="C3" s="92"/>
@@ -3193,7 +3268,7 @@
         <v>384</v>
       </c>
       <c r="E3" s="93"/>
-      <c r="F3" t="s" s="144">
+      <c r="F3" t="s" s="165">
         <v>20</v>
       </c>
       <c r="G3" s="94"/>
@@ -3201,7 +3276,7 @@
         <v>108</v>
       </c>
       <c r="I3" s="94"/>
-      <c r="J3" t="s" s="144">
+      <c r="J3" t="s" s="165">
         <v>351</v>
       </c>
       <c r="K3" s="99"/>
@@ -3266,8 +3341,8 @@
       <c r="L5" s="105"/>
       <c r="M5" s="106"/>
       <c r="N5" s="3"/>
-      <c r="O5" t="n" s="144">
-        <v>123456.0</v>
+      <c r="O5" t="n" s="165">
+        <v>123.0</v>
       </c>
       <c r="P5" s="96"/>
       <c r="Q5" s="96"/>
@@ -4146,7 +4221,7 @@
         <v>116</v>
       </c>
       <c r="F30" s="45"/>
-      <c r="G30" t="s" s="144">
+      <c r="G30" t="s" s="165">
         <v>20</v>
       </c>
       <c r="H30" s="82" t="s">

</xml_diff>